<commit_message>
Minor changes to mapping spreadsheets.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReport.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="2100" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="-26900" yWindow="6860" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Booking Report" sheetId="1" r:id="rId1"/>
@@ -402,9 +402,6 @@
     <t>/br-doc:BookingReport/j:BailBond[@structures:id=/br-doc:BookingReport/j:BailBondChargeAssociation/j:BailBond/@structures:ref]/nc:ActivityStatus/nc:StatusDescriptionText</t>
   </si>
   <si>
-    <t>/br-doc:BookingReport/j:Booking/j:BookingSubject/j:SubjectIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
     <t>/br-doc:BookingReport/j:Booking[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/nc:ActivityDate/nc:DateTime</t>
   </si>
   <si>
@@ -655,6 +652,9 @@
   </si>
   <si>
     <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/br-ext:InmateWorkerIndicator</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Booking[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:BookingSubject/j:SubjectIdentification/nc:IdentificationID</t>
   </si>
 </sst>
 </file>
@@ -773,9 +773,49 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="828">
+  <cellStyleXfs count="868">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1675,7 +1715,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="828">
+  <cellStyles count="868">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2089,6 +2129,26 @@
     <cellStyle name="Followed Hyperlink" xfId="823" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="825" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="827" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="829" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="831" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="833" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="835" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="837" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="839" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="841" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="843" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="845" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="847" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="849" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="851" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="853" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="855" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="857" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="859" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="861" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="863" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="865" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="867" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2502,6 +2562,26 @@
     <cellStyle name="Hyperlink" xfId="822" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="824" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="826" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="828" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="830" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="832" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="834" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="836" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="838" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="840" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="842" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="844" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="846" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="848" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="850" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="852" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="854" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="856" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="858" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="860" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="862" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="864" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="866" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2839,9 +2919,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E87" sqref="E87:E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2981,80 +3061,80 @@
     <row r="12" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>165</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>166</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3167,7 +3247,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
@@ -3188,86 +3268,86 @@
       </c>
     </row>
     <row r="29" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A29" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="A29" s="4"/>
       <c r="B29" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>84</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A30" s="4"/>
+      <c r="A30" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="B30" s="4" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A31" s="4"/>
       <c r="B31" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A32" s="4"/>
       <c r="B32" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A34" s="4"/>
       <c r="B34" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C34" s="4"/>
+        <v>77</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="6" customFormat="1">
       <c r="A35" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -3284,7 +3364,7 @@
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="6" customFormat="1" ht="60">
@@ -3297,7 +3377,7 @@
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="6" customFormat="1" ht="60">
@@ -3310,7 +3390,7 @@
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="6" customFormat="1" ht="60">
@@ -3323,7 +3403,7 @@
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="6" customFormat="1" ht="60">
@@ -3332,11 +3412,11 @@
         <v>1</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="6" customFormat="1">
@@ -3364,7 +3444,7 @@
         <v>16</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>125</v>
@@ -3392,7 +3472,7 @@
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
     </row>
-    <row r="46" spans="1:5" s="9" customFormat="1" ht="30">
+    <row r="46" spans="1:5" s="9" customFormat="1" ht="45">
       <c r="B46" s="21" t="s">
         <v>47</v>
       </c>
@@ -3400,7 +3480,7 @@
         <v>61</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>127</v>
+        <v>211</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3413,7 +3493,7 @@
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3426,7 +3506,7 @@
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="6" customFormat="1">
@@ -3443,7 +3523,7 @@
         <v>83</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="51" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3454,7 +3534,7 @@
         <v>40</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="6" customFormat="1">
@@ -3471,10 +3551,10 @@
         <v>96</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3485,7 +3565,7 @@
         <v>33</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3496,10 +3576,10 @@
         <v>12</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3513,7 +3593,7 @@
         <v>43</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="57" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3524,7 +3604,7 @@
         <v>35</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3535,7 +3615,7 @@
         <v>62</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3546,7 +3626,7 @@
         <v>63</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3557,7 +3637,7 @@
         <v>64</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="61" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3571,42 +3651,42 @@
         <v>66</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="62" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A62" s="5"/>
       <c r="B62" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C62" s="5" t="s">
         <v>201</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>202</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="63" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A63" s="5"/>
       <c r="B63" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="64" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A64" s="5"/>
       <c r="B64" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3621,7 +3701,7 @@
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3636,7 +3716,7 @@
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="67" spans="1:5" s="6" customFormat="1">
@@ -3656,7 +3736,7 @@
         <v>41</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="69" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3667,7 +3747,7 @@
         <v>32</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="70" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3678,7 +3758,7 @@
         <v>42</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="71" spans="1:5" s="6" customFormat="1" ht="105">
@@ -3691,7 +3771,7 @@
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="72" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3705,7 +3785,7 @@
         <v>67</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="73" spans="1:5" s="6" customFormat="1">
@@ -3720,7 +3800,7 @@
     <row r="74" spans="1:5" s="12" customFormat="1">
       <c r="A74" s="5"/>
       <c r="B74" s="20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
@@ -3729,56 +3809,56 @@
     <row r="75" spans="1:5" s="12" customFormat="1" ht="45">
       <c r="A75" s="5"/>
       <c r="B75" s="20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
       <c r="E75" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="76" spans="1:5" s="12" customFormat="1" ht="30">
       <c r="A76" s="5"/>
       <c r="B76" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
       <c r="E76" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="77" spans="1:5" s="12" customFormat="1" ht="30">
       <c r="A77" s="5"/>
       <c r="B77" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
       <c r="E77" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="78" spans="1:5" s="12" customFormat="1" ht="45">
       <c r="A78" s="5"/>
       <c r="B78" s="20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="79" spans="1:5" s="12" customFormat="1" ht="30">
       <c r="A79" s="5"/>
       <c r="B79" s="20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="80" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3789,7 +3869,7 @@
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
       <c r="E80" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="81" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3800,7 +3880,7 @@
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
       <c r="E81" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="82" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3811,12 +3891,12 @@
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
       <c r="E82" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="83" spans="1:5" s="6" customFormat="1">
       <c r="A83" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B83" s="8"/>
       <c r="C83" s="8"/>
@@ -3825,23 +3905,23 @@
     </row>
     <row r="84" spans="1:5" s="6" customFormat="1">
       <c r="B84" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="85" spans="1:5" s="6" customFormat="1">
       <c r="B85" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="30">
       <c r="A86" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B86" s="18"/>
       <c r="C86" s="18"/>
@@ -3850,56 +3930,56 @@
     </row>
     <row r="87" spans="1:5" s="15" customFormat="1" ht="30">
       <c r="B87" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D87" s="16"/>
       <c r="E87" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="88" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="B88" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D88" s="16"/>
       <c r="E88" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="89" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="B89" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D89" s="16"/>
       <c r="E89" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="90" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="B90" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D90" s="16"/>
       <c r="E90" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="91" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="B91" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D91" s="16"/>
       <c r="E91" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="B92" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D92" s="16"/>
       <c r="E92" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="93" spans="1:5" s="6" customFormat="1">

</xml_diff>

<commit_message>
Moved "HoldForAgency" to be an augmentation of "Charge" rather than "Detention.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReport.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-26900" yWindow="6860" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1700" yWindow="1180" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Booking Report" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>DOB</t>
   </si>
   <si>
-    <t>Holding for Agency</t>
-  </si>
-  <si>
     <t>Immigration Hold</t>
   </si>
   <si>
@@ -441,9 +438,6 @@
     <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/nc:ActivityDate/nc:Date</t>
   </si>
   <si>
-    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/br-ext:HoldForAgency/nc:OrganizationName</t>
-  </si>
-  <si>
     <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/br-ext:DetentiontImmigrationHoldIndicator</t>
   </si>
   <si>
@@ -655,6 +649,12 @@
   </si>
   <si>
     <t>/br-doc:BookingReport/j:Booking[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:BookingSubject/j:SubjectIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>Hold for Agency</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Charge[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/j:Charge/@structures:ref]/br-ext:HoldForAgency/nc:OrganizationName</t>
   </si>
 </sst>
 </file>
@@ -773,9 +773,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="868">
+  <cellStyleXfs count="872">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1715,7 +1719,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="868">
+  <cellStyles count="872">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2149,6 +2153,8 @@
     <cellStyle name="Followed Hyperlink" xfId="863" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="865" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="867" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="869" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="871" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2582,6 +2588,8 @@
     <cellStyle name="Hyperlink" xfId="862" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="864" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="866" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="868" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="870" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2920,8 +2928,8 @@
   <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E87" sqref="E87:E92"/>
+      <pane ySplit="2" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2935,7 +2943,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="36" customHeight="1">
       <c r="A1" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="13"/>
@@ -2953,7 +2961,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>10</v>
@@ -2961,7 +2969,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -2978,7 +2986,7 @@
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="6" customFormat="1">
@@ -2987,16 +2995,16 @@
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="6" customFormat="1">
       <c r="A6" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -3006,32 +3014,32 @@
     <row r="7" spans="1:5" s="6" customFormat="1">
       <c r="A7" s="9"/>
       <c r="B7" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="6" customFormat="1">
       <c r="A8" s="9"/>
       <c r="B8" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="6" customFormat="1">
       <c r="A9" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -3041,17 +3049,17 @@
     <row r="10" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="6" customFormat="1">
       <c r="A11" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -3061,80 +3069,80 @@
     <row r="12" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3143,11 +3151,11 @@
         <v>11</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3156,11 +3164,11 @@
         <v>2</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3169,76 +3177,76 @@
         <v>0</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3247,107 +3255,107 @@
         <v>1</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A28" s="4"/>
       <c r="B28" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A29" s="4"/>
       <c r="B29" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A30" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A31" s="4"/>
       <c r="B31" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A32" s="4"/>
       <c r="B32" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A34" s="4"/>
       <c r="B34" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="6" customFormat="1">
       <c r="A35" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -3360,50 +3368,50 @@
         <v>11</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="22" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="6" customFormat="1" ht="60">
       <c r="A37" s="3"/>
       <c r="B37" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="22" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="6" customFormat="1" ht="60">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="22" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="6" customFormat="1" ht="60">
       <c r="A39" s="3"/>
       <c r="B39" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="22" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="6" customFormat="1" ht="60">
@@ -3412,16 +3420,16 @@
         <v>1</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="22" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="6" customFormat="1">
       <c r="A41" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -3430,42 +3438,42 @@
     </row>
     <row r="42" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="B42" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="B43" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="6" customFormat="1" ht="75">
       <c r="A44" s="5"/>
       <c r="B44" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>70</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="6" customFormat="1">
       <c r="A45" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
@@ -3474,44 +3482,44 @@
     </row>
     <row r="46" spans="1:5" s="9" customFormat="1" ht="45">
       <c r="B46" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A47" s="3"/>
       <c r="B47" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A48" s="3"/>
       <c r="B48" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="6" customFormat="1">
       <c r="A49" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
@@ -3520,26 +3528,26 @@
     </row>
     <row r="50" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="B50" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="B51" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="6" customFormat="1">
       <c r="A52" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
@@ -3548,63 +3556,60 @@
     </row>
     <row r="53" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B53" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="B54" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A55" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>159</v>
+        <v>42</v>
       </c>
       <c r="E55" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B56" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E56" s="6" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A56" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E56" s="9" t="s">
+    <row r="57" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B57" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E57" s="3" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B57" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3615,83 +3620,87 @@
         <v>62</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="6" t="s">
         <v>59</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>63</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="60" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A60" s="6" t="s">
+        <v>96</v>
+      </c>
       <c r="B60" s="6" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>145</v>
+        <v>65</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="61" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A61" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>66</v>
-      </c>
+      <c r="A61" s="5"/>
+      <c r="B61" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D61" s="5"/>
       <c r="E61" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="62" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A62" s="5"/>
       <c r="B62" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>201</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="63" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A63" s="5"/>
       <c r="B63" s="5" t="s">
-        <v>166</v>
+        <v>200</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="64" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A64" s="5"/>
+      <c r="A64" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="B64" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="C64" s="5"/>
+        <v>74</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>88</v>
+      </c>
       <c r="D64" s="5"/>
       <c r="E64" s="9" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" s="6" customFormat="1" ht="45">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A65" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>75</v>
@@ -3701,96 +3710,95 @@
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="9" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="A66" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D66" s="5"/>
-      <c r="E66" s="9" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" s="6" customFormat="1">
-      <c r="A67" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B67" s="8"/>
-      <c r="C67" s="8"/>
-      <c r="D67" s="8"/>
-      <c r="E67" s="8"/>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="6" customFormat="1">
+      <c r="A66" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B66" s="8"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8"/>
+    </row>
+    <row r="67" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B67" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="68" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="B68" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="69" spans="1:5" s="6" customFormat="1" ht="30">
+    <row r="69" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B69" s="4" t="s">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="70" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B70" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C70" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E70" s="3" t="s">
+    <row r="70" spans="1:5" s="6" customFormat="1" ht="105">
+      <c r="A70" s="5"/>
+      <c r="B70" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="71" spans="1:5" s="6" customFormat="1" ht="105">
-      <c r="A71" s="5"/>
-      <c r="B71" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5" t="s">
+    <row r="71" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="A71" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E71" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="72" spans="1:5" s="6" customFormat="1" ht="30">
+    <row r="72" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A72" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>68</v>
+        <v>37</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>210</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>135</v>
+        <v>157</v>
+      </c>
+      <c r="E72" s="9" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="73" spans="1:5" s="6" customFormat="1">
       <c r="A73" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
@@ -3800,7 +3808,7 @@
     <row r="74" spans="1:5" s="12" customFormat="1">
       <c r="A74" s="5"/>
       <c r="B74" s="20" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
@@ -3809,94 +3817,94 @@
     <row r="75" spans="1:5" s="12" customFormat="1" ht="45">
       <c r="A75" s="5"/>
       <c r="B75" s="20" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
       <c r="E75" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="76" spans="1:5" s="12" customFormat="1" ht="30">
       <c r="A76" s="5"/>
       <c r="B76" s="20" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
       <c r="E76" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="77" spans="1:5" s="12" customFormat="1" ht="30">
       <c r="A77" s="5"/>
       <c r="B77" s="20" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
       <c r="E77" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="78" spans="1:5" s="12" customFormat="1" ht="45">
       <c r="A78" s="5"/>
       <c r="B78" s="20" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="79" spans="1:5" s="12" customFormat="1" ht="30">
       <c r="A79" s="5"/>
       <c r="B79" s="20" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="80" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A80" s="5"/>
       <c r="B80" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
       <c r="E80" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="81" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A81" s="5"/>
       <c r="B81" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
       <c r="E81" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="82" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A82" s="5"/>
       <c r="B82" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
       <c r="E82" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="83" spans="1:5" s="6" customFormat="1">
       <c r="A83" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B83" s="8"/>
       <c r="C83" s="8"/>
@@ -3905,23 +3913,23 @@
     </row>
     <row r="84" spans="1:5" s="6" customFormat="1">
       <c r="B84" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="85" spans="1:5" s="6" customFormat="1">
       <c r="B85" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="30">
       <c r="A86" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B86" s="18"/>
       <c r="C86" s="18"/>
@@ -3930,56 +3938,56 @@
     </row>
     <row r="87" spans="1:5" s="15" customFormat="1" ht="30">
       <c r="B87" s="15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D87" s="16"/>
       <c r="E87" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="88" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="B88" s="15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D88" s="16"/>
       <c r="E88" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="89" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="B89" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D89" s="16"/>
       <c r="E89" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="90" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="B90" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D90" s="16"/>
       <c r="E90" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="91" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="B91" s="15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D91" s="16"/>
       <c r="E91" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="B92" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D92" s="16"/>
       <c r="E92" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="93" spans="1:5" s="6" customFormat="1">

</xml_diff>

<commit_message>
Changed Booking, Custody Release, Custody Query Results and Custody Status Change to all use "BookingDetentionFacility"
Added Sex Offender, Education Occupation and Military Service Status
Code to Custody Query Results and Custody Status Change

Changed MilitaryIndicator to MilitaryServiceStatusCode across IEPDs.

Added the following to custody Release:

Age
Eye Color
Hair Color
Height
Weight
Physical Feature Description
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReport.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReport.xlsx
@@ -255,9 +255,6 @@
     <t>Occupation</t>
   </si>
   <si>
-    <t>Military Service</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sex Offender </t>
   </si>
   <si>
@@ -276,9 +273,6 @@
     <t>text to describe person occupation</t>
   </si>
   <si>
-    <t>military service experience indicator</t>
-  </si>
-  <si>
     <t>registered sex offender indicator</t>
   </si>
   <si>
@@ -378,9 +372,6 @@
     <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonAugmentation/nc:EmployeeOccupationCategoryText</t>
   </si>
   <si>
-    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonMilitarySummary/nc:MilitaryExperienceIndicator</t>
-  </si>
-  <si>
     <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonCriminalHistorySummary/j:RegisteredSexualOffenderIndicator</t>
   </si>
   <si>
@@ -655,6 +646,15 @@
   </si>
   <si>
     <t>/br-doc:BookingReport/j:Charge[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/j:Charge/@structures:ref]/br-ext:HoldForAgency/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>Military Service status Code</t>
+  </si>
+  <si>
+    <t>military service status code</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonMilitarySummary/ac-bkg-codes:MilitaryServiceStatusCode</t>
   </si>
 </sst>
 </file>
@@ -773,9 +773,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="872">
+  <cellStyleXfs count="874">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1719,7 +1721,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="872">
+  <cellStyles count="874">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2155,6 +2157,7 @@
     <cellStyle name="Followed Hyperlink" xfId="867" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="869" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="871" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="873" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2590,6 +2593,7 @@
     <cellStyle name="Hyperlink" xfId="866" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="868" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="870" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="872" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2928,8 +2932,8 @@
   <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D72" sqref="D72"/>
+      <pane ySplit="2" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2961,7 +2965,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>10</v>
@@ -2986,7 +2990,7 @@
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="6" customFormat="1">
@@ -2999,7 +3003,7 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="6" customFormat="1">
@@ -3021,7 +3025,7 @@
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="6" customFormat="1">
@@ -3034,12 +3038,12 @@
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="6" customFormat="1">
       <c r="A9" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -3049,12 +3053,12 @@
     <row r="10" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="6" customFormat="1">
@@ -3069,80 +3073,80 @@
     <row r="12" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3155,7 +3159,7 @@
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3168,7 +3172,7 @@
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3181,7 +3185,7 @@
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3194,7 +3198,7 @@
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3207,7 +3211,7 @@
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3220,7 +3224,7 @@
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3233,7 +3237,7 @@
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3246,7 +3250,7 @@
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3255,35 +3259,35 @@
         <v>1</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A28" s="4"/>
       <c r="B28" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="11" t="s">
         <v>90</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>92</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A29" s="4"/>
       <c r="B29" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3291,27 +3295,27 @@
         <v>37</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A31" s="4"/>
       <c r="B31" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3320,24 +3324,24 @@
         <v>77</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
-        <v>78</v>
+        <v>209</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>85</v>
+        <v>210</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4" t="s">
-        <v>119</v>
+        <v>211</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3346,16 +3350,16 @@
         <v>76</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="6" customFormat="1">
       <c r="A35" s="7" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -3372,7 +3376,7 @@
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="6" customFormat="1" ht="60">
@@ -3385,7 +3389,7 @@
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="22" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="6" customFormat="1" ht="60">
@@ -3398,7 +3402,7 @@
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="22" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="6" customFormat="1" ht="60">
@@ -3411,7 +3415,7 @@
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="22" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="6" customFormat="1" ht="60">
@@ -3420,11 +3424,11 @@
         <v>1</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="22" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="6" customFormat="1">
@@ -3444,7 +3448,7 @@
         <v>30</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3452,10 +3456,10 @@
         <v>15</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="6" customFormat="1" ht="75">
@@ -3468,7 +3472,7 @@
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="6" customFormat="1">
@@ -3488,20 +3492,20 @@
         <v>60</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A47" s="3"/>
       <c r="B47" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3514,7 +3518,7 @@
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="6" customFormat="1">
@@ -3528,10 +3532,10 @@
     </row>
     <row r="50" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="B50" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3542,7 +3546,7 @@
         <v>39</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="6" customFormat="1">
@@ -3556,13 +3560,13 @@
     </row>
     <row r="53" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B53" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3573,7 +3577,7 @@
         <v>32</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3587,7 +3591,7 @@
         <v>42</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3598,7 +3602,7 @@
         <v>34</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="57" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3609,7 +3613,7 @@
         <v>61</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3620,7 +3624,7 @@
         <v>62</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3631,12 +3635,12 @@
         <v>63</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="60" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A60" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>64</v>
@@ -3645,42 +3649,42 @@
         <v>65</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="61" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A61" s="5"/>
       <c r="B61" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="9" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="62" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A62" s="5"/>
       <c r="B62" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="9" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="63" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A63" s="5"/>
       <c r="B63" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="64" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3691,11 +3695,11 @@
         <v>74</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="9" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3706,11 +3710,11 @@
         <v>75</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="9" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="6" customFormat="1">
@@ -3730,7 +3734,7 @@
         <v>40</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="68" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3741,18 +3745,18 @@
         <v>31</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="69" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B69" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C69" s="6" t="s">
         <v>41</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="70" spans="1:5" s="6" customFormat="1" ht="105">
@@ -3765,7 +3769,7 @@
       </c>
       <c r="D70" s="5"/>
       <c r="E70" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="71" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3779,7 +3783,7 @@
         <v>66</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="72" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3787,18 +3791,18 @@
         <v>37</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="73" spans="1:5" s="6" customFormat="1">
       <c r="A73" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
@@ -3808,7 +3812,7 @@
     <row r="74" spans="1:5" s="12" customFormat="1">
       <c r="A74" s="5"/>
       <c r="B74" s="20" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
@@ -3817,78 +3821,78 @@
     <row r="75" spans="1:5" s="12" customFormat="1" ht="45">
       <c r="A75" s="5"/>
       <c r="B75" s="20" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
       <c r="E75" s="4" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="76" spans="1:5" s="12" customFormat="1" ht="30">
       <c r="A76" s="5"/>
       <c r="B76" s="20" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
       <c r="E76" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="77" spans="1:5" s="12" customFormat="1" ht="30">
       <c r="A77" s="5"/>
       <c r="B77" s="20" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
       <c r="E77" s="4" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="78" spans="1:5" s="12" customFormat="1" ht="45">
       <c r="A78" s="5"/>
       <c r="B78" s="20" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="79" spans="1:5" s="12" customFormat="1" ht="30">
       <c r="A79" s="5"/>
       <c r="B79" s="20" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="80" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A80" s="5"/>
       <c r="B80" s="20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
       <c r="E80" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="81" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A81" s="5"/>
       <c r="B81" s="20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
       <c r="E81" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="82" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3899,12 +3903,12 @@
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
       <c r="E82" s="4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="83" spans="1:5" s="6" customFormat="1">
       <c r="A83" s="7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B83" s="8"/>
       <c r="C83" s="8"/>
@@ -3913,23 +3917,23 @@
     </row>
     <row r="84" spans="1:5" s="6" customFormat="1">
       <c r="B84" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="85" spans="1:5" s="6" customFormat="1">
       <c r="B85" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="30">
       <c r="A86" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B86" s="18"/>
       <c r="C86" s="18"/>
@@ -3938,56 +3942,56 @@
     </row>
     <row r="87" spans="1:5" s="15" customFormat="1" ht="30">
       <c r="B87" s="15" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D87" s="16"/>
       <c r="E87" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="88" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="B88" s="15" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D88" s="16"/>
       <c r="E88" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="89" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="B89" s="15" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D89" s="16"/>
       <c r="E89" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="90" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="B90" s="15" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D90" s="16"/>
       <c r="E90" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="91" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="B91" s="15" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D91" s="16"/>
       <c r="E91" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="B92" s="15" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D92" s="16"/>
       <c r="E92" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="93" spans="1:5" s="6" customFormat="1">

</xml_diff>

<commit_message>
Added the Person_Health_Information_Search_Results to the IEPD.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReport.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="1180" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="4000" yWindow="3280" windowWidth="25600" windowHeight="13940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Booking Report" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="251">
   <si>
     <t>Race</t>
   </si>
@@ -453,9 +453,6 @@
     <t>Behavioral Health</t>
   </si>
   <si>
-    <t>Diagnosis</t>
-  </si>
-  <si>
     <t>SMI Indicator</t>
   </si>
   <si>
@@ -627,12 +624,6 @@
     <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionCondition/nc:ActivityDescriptionText</t>
   </si>
   <si>
-    <t>/br-doc:BookingReport/br-ext:BehavioralHealthInformation/j:Evaluation/j:EvaluationDiagnosisDescriptionText</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReport/br-ext:BehavioralHealthInformation/br-ext:SeriousMentalIllnessIndicator</t>
-  </si>
-  <si>
     <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/br-ext:InmateWorkReleaseIndicator</t>
   </si>
   <si>
@@ -655,6 +646,132 @@
   </si>
   <si>
     <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonMilitarySummary/ac-bkg-codes:MilitaryServiceStatusCode</t>
+  </si>
+  <si>
+    <t>HRN Indicator</t>
+  </si>
+  <si>
+    <t>Serious Mental Ilness</t>
+  </si>
+  <si>
+    <t>High Risk Needs</t>
+  </si>
+  <si>
+    <t>SA Indicator</t>
+  </si>
+  <si>
+    <t>Substance Abuse</t>
+  </si>
+  <si>
+    <t>GMHC Indicatior</t>
+  </si>
+  <si>
+    <t>General Mental Health Condition</t>
+  </si>
+  <si>
+    <t>Diagnosis Description</t>
+  </si>
+  <si>
+    <t>Treatment Start Date</t>
+  </si>
+  <si>
+    <t>Treatment End Date</t>
+  </si>
+  <si>
+    <t>Treatment Provider</t>
+  </si>
+  <si>
+    <t>TCO Indicator</t>
+  </si>
+  <si>
+    <t>Treeatment Court Ordered</t>
+  </si>
+  <si>
+    <t>TA Indicator</t>
+  </si>
+  <si>
+    <t>Treatment Active Indicator</t>
+  </si>
+  <si>
+    <t>Prescribed Medication Name</t>
+  </si>
+  <si>
+    <t>Medication Product ID</t>
+  </si>
+  <si>
+    <t>Medication Dispensing Date</t>
+  </si>
+  <si>
+    <t>Medication Dose Text</t>
+  </si>
+  <si>
+    <t>Medicaid Indicator</t>
+  </si>
+  <si>
+    <t>Regional Behavioral Health Authority Assigment Text</t>
+  </si>
+  <si>
+    <t>Care Episode</t>
+  </si>
+  <si>
+    <t>Care EpisodeStart Date</t>
+  </si>
+  <si>
+    <t>Care Episode End Date</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/br-ext:BehavioralHealthInformation[@structures:id=/br-doc:BookingReport/nc:Person/br-ext:PersonBehavioralHealthInformation/@structures:ref]/br-ext:SeriousMentalIllnessIndicator</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/br-ext:BehavioralHealthInformation[@structures:id=/br-doc:BookingReport/nc:Person/br-ext:PersonBehavioralHealthInformation/@structures:ref]/br-ext:HighRiskNeedsIndicator</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/br-ext:BehavioralHealthInformation[@structures:id=/br-doc:BookingReport/nc:Person/br-ext:PersonBehavioralHealthInformation/@structures:ref]/br-ext:SubstanceAbuseIndicator</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/br-ext:BehavioralHealthInformation[@structures:id=/br-doc:BookingReport/nc:Person/br-ext:PersonBehavioralHealthInformation/@structures:ref]/br-ext:GeneralMentalHealthConditionIndicator</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/br-ext:BehavioralHealthInformation[@structures:id=/br-doc:BookingReport/nc:Person/br-ext:PersonBehavioralHealthInformation/@structures:ref]/j:Evaluation/j:EvaluationDiagnosisDescriptionText</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/br-ext:BehavioralHealthInformation[@structures:id=/br-doc:BookingReport/nc:Person/br-ext:PersonBehavioralHealthInformation/@structures:ref]/nc:Treatment/nc:ActivityDateRange/nc:StartDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/br-ext:BehavioralHealthInformation[@structures:id=/br-doc:BookingReport/nc:Person/br-ext:PersonBehavioralHealthInformation/@structures:ref]/nc:Treatment/nc:ActivityDateRange/nc:EndDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/br-ext:BehavioralHealthInformation[@structures:id=/br-doc:BookingReport/nc:Person/br-ext:PersonBehavioralHealthInformation/@structures:ref]/nc:Treatment/nc:TreatmentProvider/nc:EntityOrganization/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/br-ext:BehavioralHealthInformation[@structures:id=/br-doc:BookingReport/nc:Person/br-ext:PersonBehavioralHealthInformation/@structures:ref]/nc:Treatment/br-ext:TreatmentCourtOrderedIndicator</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/br-ext:BehavioralHealthInformation[@structures:id=/br-doc:BookingReport/nc:Person/br-ext:PersonBehavioralHealthInformation/@structures:ref]/nc:Treatment/br-ext:TreatmentActiveIndicator</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/br-ext:BehavioralHealthInformation[@structures:id=/br-doc:BookingReport/nc:Person/br-ext:PersonBehavioralHealthInformation/@structures:ref]/br-ext:PrescribedMedication/cyfs:Medication/nc:ItemName</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/br-ext:BehavioralHealthInformation[@structures:id=/br-doc:BookingReport/nc:Person/br-ext:PersonBehavioralHealthInformation/@structures:ref]/br-ext:PrescribedMedication/cyfs:Medication/br-ext:MedicationGeneralProductIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/br-ext:BehavioralHealthInformation[@structures:id=/br-doc:BookingReport/nc:Person/br-ext:PersonBehavioralHealthInformation/@structures:ref]/br-ext:PrescribedMedication/cyfs:MedicationDispensingDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/br-ext:BehavioralHealthInformation[@structures:id=/br-doc:BookingReport/nc:Person/br-ext:PersonBehavioralHealthInformation/@structures:ref]/br-ext:PrescribedMedication/cyfs:MedicationDoseMeasure/nc:MeasureValueText</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/br-ext:BehavioralHealthInformation[@structures:id=/br-doc:BookingReport/nc:Person/br-ext:PersonBehavioralHealthInformation/@structures:ref]/br-ext:RegionalBehavioralHealthAuthorityAssignmentText</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/br-ext:BehavioralHealthInformation[@structures:id=/br-doc:BookingReport/nc:Person/br-ext:PersonBehavioralHealthInformation/@structures:ref]/hs:MedicaidIndicator</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/br-ext:CareEpisode[@structures:id=/br-doc:BookingReport/nc:Person/br-ext:PersonCareEpisode/@structures:ref]/nc:ActivityDateRange/nc:StartDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/br-ext:CareEpisode[@structures:id=/br-doc:BookingReport/nc:Person/br-ext:PersonCareEpisode/@structures:ref]/nc:ActivityDateRange/nc:EndDate/nc:Date</t>
   </si>
 </sst>
 </file>
@@ -773,9 +890,37 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="874">
+  <cellStyleXfs count="902">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1721,7 +1866,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="874">
+  <cellStyles count="902">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2158,6 +2303,20 @@
     <cellStyle name="Followed Hyperlink" xfId="869" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="871" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="873" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="875" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="877" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="879" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="881" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="883" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="885" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="887" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="889" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="891" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="893" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="895" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="897" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="899" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="901" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2594,6 +2753,20 @@
     <cellStyle name="Hyperlink" xfId="868" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="870" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="872" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="874" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="876" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="878" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="880" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="882" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="884" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="886" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="888" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="890" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="892" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="894" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="896" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="898" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="900" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2929,11 +3102,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:E119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
+      <pane ySplit="2" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3078,75 +3251,75 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>159</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>160</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3259,7 +3432,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
@@ -3334,14 +3507,14 @@
     <row r="33" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3376,7 +3549,7 @@
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="6" customFormat="1" ht="60">
@@ -3389,7 +3562,7 @@
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="6" customFormat="1" ht="60">
@@ -3402,7 +3575,7 @@
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="6" customFormat="1" ht="60">
@@ -3415,7 +3588,7 @@
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="6" customFormat="1" ht="60">
@@ -3424,11 +3597,11 @@
         <v>1</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="6" customFormat="1">
@@ -3456,7 +3629,7 @@
         <v>15</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>121</v>
@@ -3492,7 +3665,7 @@
         <v>60</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3563,7 +3736,7 @@
         <v>93</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>134</v>
@@ -3649,42 +3822,42 @@
         <v>65</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="61" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A61" s="5"/>
       <c r="B61" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C61" s="5" t="s">
         <v>195</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>196</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="62" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A62" s="5"/>
       <c r="B62" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="63" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A63" s="5"/>
       <c r="B63" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="64" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3699,7 +3872,7 @@
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3714,7 +3887,7 @@
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="9" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="6" customFormat="1">
@@ -3791,13 +3964,13 @@
         <v>37</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="73" spans="1:5" s="6" customFormat="1">
@@ -3812,7 +3985,7 @@
     <row r="74" spans="1:5" s="12" customFormat="1">
       <c r="A74" s="5"/>
       <c r="B74" s="20" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
@@ -3821,56 +3994,56 @@
     <row r="75" spans="1:5" s="12" customFormat="1" ht="45">
       <c r="A75" s="5"/>
       <c r="B75" s="20" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
       <c r="E75" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="76" spans="1:5" s="12" customFormat="1" ht="30">
       <c r="A76" s="5"/>
       <c r="B76" s="20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
       <c r="E76" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="77" spans="1:5" s="12" customFormat="1" ht="30">
       <c r="A77" s="5"/>
       <c r="B77" s="20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
       <c r="E77" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="78" spans="1:5" s="12" customFormat="1" ht="45">
       <c r="A78" s="5"/>
       <c r="B78" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="79" spans="1:5" s="12" customFormat="1" ht="30">
       <c r="A79" s="5"/>
       <c r="B79" s="20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="80" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3903,7 +4076,7 @@
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
       <c r="E82" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="83" spans="1:5" s="6" customFormat="1">
@@ -3915,97 +4088,252 @@
       <c r="D83" s="8"/>
       <c r="E83" s="8"/>
     </row>
-    <row r="84" spans="1:5" s="6" customFormat="1">
+    <row r="84" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B84" s="6" t="s">
         <v>144</v>
       </c>
+      <c r="C84" s="6" t="s">
+        <v>210</v>
+      </c>
       <c r="E84" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" s="6" customFormat="1">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B85" s="4" t="s">
-        <v>145</v>
+        <v>209</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>211</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="30">
-      <c r="A86" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B86" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B87" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B88" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" s="6" customFormat="1" ht="60">
+      <c r="B89" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" s="6" customFormat="1" ht="60">
+      <c r="B90" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" s="6" customFormat="1" ht="60">
+      <c r="B91" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B92" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B93" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B94" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B95" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B96" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B97" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B98" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B99" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" s="6" customFormat="1">
+      <c r="A100" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B100" s="8"/>
+      <c r="C100" s="8"/>
+      <c r="D100" s="8"/>
+      <c r="E100" s="8"/>
+    </row>
+    <row r="101" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B101" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B102" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="30">
+      <c r="A103" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B103" s="18"/>
+      <c r="C103" s="18"/>
+      <c r="D103" s="14"/>
+      <c r="E103" s="19"/>
+    </row>
+    <row r="104" spans="1:5" s="15" customFormat="1" ht="30">
+      <c r="B104" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="D104" s="16"/>
+      <c r="E104" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" s="15" customFormat="1" ht="45">
+      <c r="B105" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D105" s="16"/>
+      <c r="E105" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" s="15" customFormat="1" ht="45">
+      <c r="B106" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="D106" s="16"/>
+      <c r="E106" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" s="15" customFormat="1" ht="45">
+      <c r="B107" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="D107" s="16"/>
+      <c r="E107" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" s="15" customFormat="1" ht="45">
+      <c r="B108" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="B86" s="18"/>
-      <c r="C86" s="18"/>
-      <c r="D86" s="14"/>
-      <c r="E86" s="19"/>
-    </row>
-    <row r="87" spans="1:5" s="15" customFormat="1" ht="30">
-      <c r="B87" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="D87" s="16"/>
-      <c r="E87" s="3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" s="15" customFormat="1" ht="45">
-      <c r="B88" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="D88" s="16"/>
-      <c r="E88" s="3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" s="15" customFormat="1" ht="45">
-      <c r="B89" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="D89" s="16"/>
-      <c r="E89" s="3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" s="15" customFormat="1" ht="45">
-      <c r="B90" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="D90" s="16"/>
-      <c r="E90" s="3" t="s">
+      <c r="D108" s="16"/>
+      <c r="E108" s="3" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="91" spans="1:5" s="15" customFormat="1" ht="45">
-      <c r="B91" s="15" t="s">
+    <row r="109" spans="1:5" s="15" customFormat="1" ht="45">
+      <c r="B109" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="D91" s="16"/>
-      <c r="E91" s="3" t="s">
+      <c r="D109" s="16"/>
+      <c r="E109" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="92" spans="1:5" s="15" customFormat="1" ht="45">
-      <c r="B92" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="D92" s="16"/>
-      <c r="E92" s="3" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" s="6" customFormat="1">
-      <c r="E93" s="9"/>
-    </row>
-    <row r="94" spans="1:5" s="6" customFormat="1"/>
-    <row r="95" spans="1:5" s="6" customFormat="1"/>
-    <row r="96" spans="1:5" s="6" customFormat="1"/>
-    <row r="97" s="6" customFormat="1"/>
-    <row r="98" s="6" customFormat="1"/>
-    <row r="99" s="6" customFormat="1"/>
-    <row r="100" s="6" customFormat="1"/>
-    <row r="101" s="6" customFormat="1"/>
-    <row r="102" s="6" customFormat="1"/>
+    <row r="110" spans="1:5" s="6" customFormat="1">
+      <c r="E110" s="9"/>
+    </row>
+    <row r="111" spans="1:5" s="6" customFormat="1"/>
+    <row r="112" spans="1:5" s="6" customFormat="1"/>
+    <row r="113" s="6" customFormat="1"/>
+    <row r="114" s="6" customFormat="1"/>
+    <row r="115" s="6" customFormat="1"/>
+    <row r="116" s="6" customFormat="1"/>
+    <row r="117" s="6" customFormat="1"/>
+    <row r="118" s="6" customFormat="1"/>
+    <row r="119" s="6" customFormat="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Added an XML Instance with multiple arrests/charges/etc.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReport.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4000" yWindow="3280" windowWidth="25600" windowHeight="13940" tabRatio="500"/>
+    <workbookView xWindow="2560" yWindow="980" windowWidth="26800" windowHeight="13940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Booking Report" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="250">
   <si>
     <t>Race</t>
   </si>
@@ -333,9 +333,6 @@
     <t>/br-doc:BookingReport/intel:SystemIdentification/nc:SystemName</t>
   </si>
   <si>
-    <t>/br-doc:BookingReport/nc:Case[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:CaseAugmentation/j:CaseCourt/j:CourtName</t>
-  </si>
-  <si>
     <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonBirthDate/nc:Date</t>
   </si>
   <si>
@@ -390,60 +387,18 @@
     <t>/br-doc:BookingReport/j:BailBond[@structures:id=/br-doc:BookingReport/j:BailBondChargeAssociation/j:BailBond/@structures:ref]/nc:ActivityStatus/nc:StatusDescriptionText</t>
   </si>
   <si>
-    <t>/br-doc:BookingReport/j:Booking[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/nc:ActivityDate/nc:DateTime</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReport/j:Booking[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:BookingDetentionFacility/nc:FacilityIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
     <t>/br-doc:BookingReport/cyfs:NextCourtEvent[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:CourtEventCourt/j:CourtName</t>
   </si>
   <si>
     <t>/br-doc:BookingReport/cyfs:NextCourtEvent[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/nc:ActivityDate/nc:Date</t>
   </si>
   <si>
-    <t>/br-doc:BookingReport/j:Charge[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/j:Charge/@structures:ref]/j:ChargeSequenceID</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReport/j:Charge[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/j:Charge/@structures:ref]/j:ChargeDescriptionText</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReport/j:Charge[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/j:Charge/@structures:ref]/j:ChargeStatute/j:StatuteCodeSectionIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /br-doc:BookingReport/j:Charge[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/j:Charge/@structures:ref]/j:ChargeCategoryDescriptionText</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReport/j:Charge[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/j:Charge/@structures:ref]/j:ChargeHighestIndicator</t>
-  </si>
-  <si>
     <t>/br-doc:BookingReport/nc:Location[@structures:id=/br-doc:BookingReport/j:Arrest/j:ArrestLocation/@structures:ref]/nc:Location2DGeospatialCoordinate/nc:GeographicCoordinateLatitude/nc:LatitudeDegreeValue</t>
   </si>
   <si>
     <t>/br-doc:BookingReport/nc:Location[@structures:id=/br-doc:BookingReport/j:Arrest/j:ArrestLocation/@structures:ref]/nc:Location2DGeospatialCoordinate/nc:GeographicCoordinateLongitude/nc:LongitudeDegreeValue</t>
   </si>
   <si>
-    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionReleaseDate/nc:DateTime</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/nc:ActivityDate/nc:Date</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/br-ext:DetentiontImmigrationHoldIndicator</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionReleaseDate/nc:Date</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionAreaIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionBedIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionCellIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
     <t>Alias</t>
   </si>
   <si>
@@ -567,9 +522,6 @@
     <t>/br-doc:BookingReport/nc:ContactInformation[@structures:id=/br-doc:BookingReport/nc:ContactInformationAssociation/nc:ContactInformation/@structures:ref]/nc:ContactEmailID</t>
   </si>
   <si>
-    <t>Arrest Location - Apt/Suite</t>
-  </si>
-  <si>
     <t>Arrest Location - Street Number</t>
   </si>
   <si>
@@ -600,9 +552,6 @@
     <t>/br-doc:BookingReport/nc:Location[@structures:id=/br-doc:BookingReport/j:Arrest/j:ArrestLocation/@structures:ref]/nc:Address/nc:LocationPostalCode</t>
   </si>
   <si>
-    <t>/br-doc:BookingReport/j:Arrest[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:ArrestAgency/nc:OrganizationName</t>
-  </si>
-  <si>
     <t>PreTrial Status (Case/Custody Status)</t>
   </si>
   <si>
@@ -612,33 +561,9 @@
     <t>Supervision Condition</t>
   </si>
   <si>
-    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionBedIdentification/ac-bkg-codes:BedCategoryCode</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/nc:SupervisionCustodyStatus/nc:StatusDescriptionText</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/br-ext:AllowAccountDepositIndicator</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionCondition/nc:ActivityDescriptionText</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/br-ext:InmateWorkReleaseIndicator</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/br-ext:InmateWorkerIndicator</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReport/j:Booking[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:BookingSubject/j:SubjectIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
     <t>Hold for Agency</t>
   </si>
   <si>
-    <t>/br-doc:BookingReport/j:Charge[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/j:Charge/@structures:ref]/br-ext:HoldForAgency/nc:OrganizationName</t>
-  </si>
-  <si>
     <t>Military Service status Code</t>
   </si>
   <si>
@@ -772,6 +697,78 @@
   </si>
   <si>
     <t>/br-doc:BookingReport/br-ext:CareEpisode[@structures:id=/br-doc:BookingReport/nc:Person/br-ext:PersonCareEpisode/@structures:ref]/nc:ActivityDateRange/nc:EndDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Case[@structures:id=/br-doc:BookingReport/j:ActivityCaseAssociation/nc:Case/@structures:ref]/j:CaseAugmentation/j:CaseCourt/j:CourtName</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Booking[@structures:id=/br-doc:BookingReport/j:ActivityCaseAssociation/nc:Activity/@structures:ref]/j:BookingSubject/j:SubjectIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Booking[@structures:id=/br-doc:BookingReport/j:ActivityCaseAssociation/nc:Activity/@structures:ref]/nc:ActivityDate/nc:DateTime</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Booking[@structures:id=/br-doc:BookingReport/j:ActivityCaseAssociation/nc:Activity/@structures:ref]/j:BookingDetentionFacility/nc:FacilityIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityCaseAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionReleaseDate/nc:DateTime</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityCaseAssociation/nc:Activity/@structures:ref]/nc:ActivityDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityCaseAssociation/nc:Activity/@structures:ref]/br-ext:DetentiontImmigrationHoldIndicator</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityCaseAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionReleaseDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityCaseAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionAreaIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityCaseAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionBedIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityCaseAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionCellIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityCaseAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionBedIdentification/ac-bkg-codes:BedCategoryCode</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityCaseAssociation/nc:Activity/@structures:ref]/nc:SupervisionCustodyStatus/nc:StatusDescriptionText</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityCaseAssociation/nc:Activity/@structures:ref]/br-ext:AllowAccountDepositIndicator</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityCaseAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionCondition/nc:ActivityDescriptionText</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityCaseAssociation/nc:Activity/@structures:ref]/br-ext:InmateWorkReleaseIndicator</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityCaseAssociation/nc:Activity/@structures:ref]/br-ext:InmateWorkerIndicator</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Arrest[@structures:id=/br-doc:BookingReport/j:Booking/j:Arrest/@structures:ref]/j:ArrestAgency/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Charge[@structures:id=/br-doc:BookingReport/j:Arrest/j:ArrestCharge/@structures:ref]/j:ChargeSequenceID</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Charge[@structures:id=/br-doc:BookingReport/j:Arrest/j:ArrestCharge/@structures:ref]/j:ChargeDescriptionText</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Charge[@structures:id=/br-doc:BookingReport/j:Arrest/j:ArrestCharge/@structures:ref]/j:ChargeStatute/j:StatuteCodeSectionIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /br-doc:BookingReport/j:Charge[@structures:id=/br-doc:BookingReport/j:Arrest/j:ArrestCharge/@structures:ref]/j:ChargeCategoryDescriptionText</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Charge[@structures:id=/br-doc:BookingReport/j:Arrest/j:ArrestCharge/@structures:ref]/j:ChargeHighestIndicator</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Charge[@structures:id=/br-doc:BookingReport/j:Arrest/j:ArrestCharge/@structures:ref]/br-ext:HoldForAgency/nc:OrganizationName</t>
   </si>
 </sst>
 </file>
@@ -3102,11 +3099,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E119"/>
+  <dimension ref="A1:E118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D99" sqref="D99"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A74" sqref="A74:XFD74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3231,7 +3228,7 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>104</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="6" customFormat="1">
@@ -3246,80 +3243,80 @@
     <row r="12" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3332,7 +3329,7 @@
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3345,7 +3342,7 @@
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3358,7 +3355,7 @@
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3371,7 +3368,7 @@
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3384,7 +3381,7 @@
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3397,7 +3394,7 @@
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3410,7 +3407,7 @@
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3423,7 +3420,7 @@
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3432,11 +3429,11 @@
         <v>1</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3449,7 +3446,7 @@
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3460,7 +3457,7 @@
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3475,7 +3472,7 @@
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3488,7 +3485,7 @@
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3501,20 +3498,20 @@
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>207</v>
+        <v>182</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4" t="s">
-        <v>208</v>
+        <v>183</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3527,12 +3524,12 @@
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="6" customFormat="1">
       <c r="A35" s="7" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -3549,7 +3546,7 @@
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="22" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="6" customFormat="1" ht="60">
@@ -3562,7 +3559,7 @@
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="22" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="6" customFormat="1" ht="60">
@@ -3575,7 +3572,7 @@
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="22" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="6" customFormat="1" ht="60">
@@ -3588,7 +3585,7 @@
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="22" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="6" customFormat="1" ht="60">
@@ -3597,11 +3594,11 @@
         <v>1</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="22" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="6" customFormat="1">
@@ -3621,7 +3618,7 @@
         <v>30</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3629,10 +3626,10 @@
         <v>15</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="6" customFormat="1" ht="75">
@@ -3645,7 +3642,7 @@
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="6" customFormat="1">
@@ -3665,7 +3662,7 @@
         <v>60</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3678,7 +3675,7 @@
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3" t="s">
-        <v>123</v>
+        <v>228</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3691,7 +3688,7 @@
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3" t="s">
-        <v>124</v>
+        <v>229</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="6" customFormat="1">
@@ -3708,7 +3705,7 @@
         <v>81</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="51" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3719,7 +3716,7 @@
         <v>39</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="6" customFormat="1">
@@ -3736,10 +3733,10 @@
         <v>93</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>134</v>
+        <v>230</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3750,7 +3747,7 @@
         <v>32</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>135</v>
+        <v>231</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3764,7 +3761,7 @@
         <v>42</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>136</v>
+        <v>232</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3775,7 +3772,7 @@
         <v>34</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>137</v>
+        <v>233</v>
       </c>
     </row>
     <row r="57" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3786,7 +3783,7 @@
         <v>61</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>138</v>
+        <v>234</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3797,7 +3794,7 @@
         <v>62</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>139</v>
+        <v>235</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3808,7 +3805,7 @@
         <v>63</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>140</v>
+        <v>236</v>
       </c>
     </row>
     <row r="60" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3822,45 +3819,45 @@
         <v>65</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>197</v>
+        <v>237</v>
       </c>
     </row>
     <row r="61" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A61" s="5"/>
       <c r="B61" s="5" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="9" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
     </row>
     <row r="62" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A62" s="5"/>
       <c r="B62" s="5" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="9" t="s">
-        <v>199</v>
+        <v>239</v>
       </c>
     </row>
     <row r="63" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A63" s="5"/>
       <c r="B63" s="5" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="9" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" s="6" customFormat="1" ht="45">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A64" s="5" t="s">
         <v>37</v>
       </c>
@@ -3872,7 +3869,7 @@
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="9" t="s">
-        <v>201</v>
+        <v>241</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3887,7 +3884,7 @@
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="9" t="s">
-        <v>202</v>
+        <v>242</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="6" customFormat="1">
@@ -3907,7 +3904,7 @@
         <v>40</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>127</v>
+        <v>244</v>
       </c>
     </row>
     <row r="68" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3918,7 +3915,7 @@
         <v>31</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>128</v>
+        <v>245</v>
       </c>
     </row>
     <row r="69" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3929,7 +3926,7 @@
         <v>41</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>129</v>
+        <v>246</v>
       </c>
     </row>
     <row r="70" spans="1:5" s="6" customFormat="1" ht="105">
@@ -3942,7 +3939,7 @@
       </c>
       <c r="D70" s="5"/>
       <c r="E70" s="5" t="s">
-        <v>130</v>
+        <v>247</v>
       </c>
     </row>
     <row r="71" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3956,21 +3953,21 @@
         <v>66</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" s="6" customFormat="1" ht="45">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A72" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>205</v>
+        <v>249</v>
       </c>
     </row>
     <row r="73" spans="1:5" s="6" customFormat="1">
@@ -3982,349 +3979,341 @@
       <c r="D73" s="8"/>
       <c r="E73" s="8"/>
     </row>
-    <row r="74" spans="1:5" s="12" customFormat="1">
+    <row r="74" spans="1:5" s="12" customFormat="1" ht="45">
       <c r="A74" s="5"/>
       <c r="B74" s="20" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
-      <c r="E74" s="4"/>
-    </row>
-    <row r="75" spans="1:5" s="12" customFormat="1" ht="45">
+      <c r="E74" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" s="12" customFormat="1" ht="30">
       <c r="A75" s="5"/>
       <c r="B75" s="20" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
       <c r="E75" s="4" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
     </row>
     <row r="76" spans="1:5" s="12" customFormat="1" ht="30">
       <c r="A76" s="5"/>
       <c r="B76" s="20" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
       <c r="E76" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" s="12" customFormat="1" ht="30">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" s="12" customFormat="1" ht="45">
       <c r="A77" s="5"/>
       <c r="B77" s="20" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
       <c r="E77" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" s="12" customFormat="1" ht="45">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" s="12" customFormat="1" ht="30">
       <c r="A78" s="5"/>
       <c r="B78" s="20" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" s="12" customFormat="1" ht="30">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A79" s="5"/>
       <c r="B79" s="20" t="s">
-        <v>187</v>
+        <v>96</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="4" t="s">
-        <v>192</v>
+        <v>124</v>
       </c>
     </row>
     <row r="80" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A80" s="5"/>
       <c r="B80" s="20" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
       <c r="E80" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" s="6" customFormat="1" ht="45">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A81" s="5"/>
-      <c r="B81" s="20" t="s">
-        <v>97</v>
+      <c r="B81" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
       <c r="E81" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A82" s="5"/>
-      <c r="B82" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C82" s="5"/>
-      <c r="D82" s="5"/>
-      <c r="E82" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" s="6" customFormat="1">
-      <c r="A83" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="B83" s="8"/>
-      <c r="C83" s="8"/>
-      <c r="D83" s="8"/>
-      <c r="E83" s="8"/>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" s="6" customFormat="1">
+      <c r="A82" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B82" s="8"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="8"/>
+    </row>
+    <row r="83" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B83" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="84" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B84" s="6" t="s">
-        <v>144</v>
+      <c r="B84" s="4" t="s">
+        <v>184</v>
       </c>
       <c r="C84" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B85" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="E85" s="3" t="s">
         <v>210</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B85" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="86" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B86" s="6" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>235</v>
+        <v>211</v>
       </c>
     </row>
     <row r="87" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B87" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>215</v>
+        <v>191</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" s="6" customFormat="1" ht="45">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" s="6" customFormat="1" ht="60">
       <c r="B88" s="6" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>237</v>
+        <v>213</v>
       </c>
     </row>
     <row r="89" spans="1:5" s="6" customFormat="1" ht="60">
       <c r="B89" s="6" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
     </row>
     <row r="90" spans="1:5" s="6" customFormat="1" ht="60">
       <c r="B90" s="6" t="s">
-        <v>218</v>
+        <v>194</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" s="6" customFormat="1" ht="60">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B91" s="6" t="s">
-        <v>219</v>
+        <v>195</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B92" s="6" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>221</v>
+        <v>198</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>241</v>
+        <v>217</v>
       </c>
     </row>
     <row r="93" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B93" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>242</v>
+        <v>218</v>
       </c>
     </row>
     <row r="94" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B94" s="6" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
     </row>
     <row r="95" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B95" s="6" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>244</v>
+        <v>220</v>
       </c>
     </row>
     <row r="96" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B96" s="6" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>245</v>
+        <v>221</v>
       </c>
     </row>
     <row r="97" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B97" s="6" t="s">
-        <v>227</v>
+      <c r="B97" s="4" t="s">
+        <v>203</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>246</v>
+        <v>223</v>
       </c>
     </row>
     <row r="98" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B98" s="4" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B99" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="E99" s="3" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" s="6" customFormat="1">
-      <c r="A100" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="B100" s="8"/>
-      <c r="C100" s="8"/>
-      <c r="D100" s="8"/>
-      <c r="E100" s="8"/>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" s="6" customFormat="1">
+      <c r="A99" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="B99" s="8"/>
+      <c r="C99" s="8"/>
+      <c r="D99" s="8"/>
+      <c r="E99" s="8"/>
+    </row>
+    <row r="100" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B100" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="101" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B101" s="6" t="s">
-        <v>231</v>
+      <c r="B101" s="4" t="s">
+        <v>207</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B102" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="E102" s="3" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" ht="30">
-      <c r="A103" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B103" s="18"/>
-      <c r="C103" s="18"/>
-      <c r="D103" s="14"/>
-      <c r="E103" s="19"/>
-    </row>
-    <row r="104" spans="1:5" s="15" customFormat="1" ht="30">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="30">
+      <c r="A102" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B102" s="18"/>
+      <c r="C102" s="18"/>
+      <c r="D102" s="14"/>
+      <c r="E102" s="19"/>
+    </row>
+    <row r="103" spans="1:5" s="15" customFormat="1" ht="30">
+      <c r="B103" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D103" s="16"/>
+      <c r="E103" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="B104" s="15" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="D104" s="16"/>
       <c r="E104" s="3" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
     </row>
     <row r="105" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="B105" s="15" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="D105" s="16"/>
       <c r="E105" s="3" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
     </row>
     <row r="106" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="B106" s="15" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="D106" s="16"/>
       <c r="E106" s="3" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
     </row>
     <row r="107" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="B107" s="15" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="D107" s="16"/>
       <c r="E107" s="3" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
     </row>
     <row r="108" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="B108" s="15" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="D108" s="16"/>
       <c r="E108" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" s="15" customFormat="1" ht="45">
-      <c r="B109" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="D109" s="16"/>
-      <c r="E109" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" s="6" customFormat="1">
-      <c r="E110" s="9"/>
-    </row>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" s="6" customFormat="1">
+      <c r="E109" s="9"/>
+    </row>
+    <row r="110" spans="1:5" s="6" customFormat="1"/>
     <row r="111" spans="1:5" s="6" customFormat="1"/>
     <row r="112" spans="1:5" s="6" customFormat="1"/>
     <row r="113" s="6" customFormat="1"/>
@@ -4333,7 +4322,6 @@
     <row r="116" s="6" customFormat="1"/>
     <row r="117" s="6" customFormat="1"/>
     <row r="118" s="6" customFormat="1"/>
-    <row r="119" s="6" customFormat="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Added Scheduled Release Date
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReport.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReport.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="980" windowWidth="26800" windowHeight="13940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="1125" windowWidth="17595" windowHeight="8505" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Booking Report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="252">
   <si>
     <t>Race</t>
   </si>
@@ -769,6 +769,12 @@
   </si>
   <si>
     <t>/br-doc:BookingReport/j:Charge[@structures:id=/br-doc:BookingReport/j:Arrest/j:ArrestCharge/@structures:ref]/br-ext:HoldForAgency/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>Supervision Scheduled  Release Date</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityCaseAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionReleaseEligibilityDate/nc:Date</t>
   </si>
 </sst>
 </file>
@@ -3099,23 +3105,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E118"/>
+  <dimension ref="A1:E119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A74" sqref="A74:XFD74"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="17" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" style="17" customWidth="1"/>
-    <col min="3" max="4" width="28.33203125" style="17" customWidth="1"/>
-    <col min="5" max="5" width="92.33203125" style="17" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="17"/>
+    <col min="1" max="1" width="20.375" style="17" customWidth="1"/>
+    <col min="2" max="2" width="27.625" style="17" customWidth="1"/>
+    <col min="3" max="4" width="28.375" style="17" customWidth="1"/>
+    <col min="5" max="5" width="92.375" style="17" customWidth="1"/>
+    <col min="6" max="16384" width="10.875" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="36" customHeight="1">
+    <row r="1" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>43</v>
       </c>
@@ -3124,7 +3130,7 @@
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
     </row>
-    <row r="2" spans="1:5" ht="36" customHeight="1">
+    <row r="2" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -3141,7 +3147,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
@@ -3150,7 +3156,7 @@
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
     </row>
-    <row r="4" spans="1:5" s="6" customFormat="1" ht="30">
+    <row r="4" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>7</v>
@@ -3163,7 +3169,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="6" customFormat="1">
+    <row r="5" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
         <v>5</v>
@@ -3176,7 +3182,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="6" customFormat="1">
+    <row r="6" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>45</v>
       </c>
@@ -3185,7 +3191,7 @@
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" spans="1:5" s="6" customFormat="1">
+    <row r="7" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9" t="s">
         <v>23</v>
@@ -3198,7 +3204,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="6" customFormat="1">
+    <row r="8" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="9" t="s">
         <v>24</v>
@@ -3211,7 +3217,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="6" customFormat="1">
+    <row r="9" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>98</v>
       </c>
@@ -3220,7 +3226,7 @@
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:5" s="6" customFormat="1" ht="45">
+    <row r="10" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
         <v>99</v>
@@ -3231,7 +3237,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="6" customFormat="1">
+    <row r="11" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>44</v>
       </c>
@@ -3240,7 +3246,7 @@
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:5" s="6" customFormat="1" ht="45">
+    <row r="12" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
         <v>127</v>
@@ -3251,7 +3257,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="6" customFormat="1" ht="45">
+    <row r="13" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
         <v>150</v>
@@ -3262,7 +3268,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="6" customFormat="1" ht="30">
+    <row r="14" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
         <v>139</v>
@@ -3273,7 +3279,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="6" customFormat="1" ht="30">
+    <row r="15" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
         <v>140</v>
@@ -3284,7 +3290,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="6" customFormat="1" ht="45">
+    <row r="16" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
         <v>141</v>
@@ -3295,7 +3301,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="6" customFormat="1" ht="45">
+    <row r="17" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
         <v>142</v>
@@ -3306,7 +3312,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="6" customFormat="1" ht="45">
+    <row r="18" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
         <v>143</v>
@@ -3319,7 +3325,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="6" customFormat="1" ht="30">
+    <row r="19" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
         <v>11</v>
@@ -3332,7 +3338,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="6" customFormat="1" ht="30">
+    <row r="20" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
         <v>2</v>
@@ -3345,7 +3351,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="6" customFormat="1" ht="30">
+    <row r="21" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
         <v>0</v>
@@ -3358,7 +3364,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="6" customFormat="1" ht="45">
+    <row r="22" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
         <v>47</v>
@@ -3371,7 +3377,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="6" customFormat="1" ht="45">
+    <row r="23" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
         <v>50</v>
@@ -3384,7 +3390,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="6" customFormat="1" ht="45">
+    <row r="24" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
         <v>54</v>
@@ -3397,7 +3403,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="6" customFormat="1" ht="45">
+    <row r="25" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
         <v>55</v>
@@ -3410,7 +3416,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="6" customFormat="1" ht="45">
+    <row r="26" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
         <v>56</v>
@@ -3423,7 +3429,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="6" customFormat="1" ht="30">
+    <row r="27" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
         <v>1</v>
@@ -3436,7 +3442,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="6" customFormat="1" ht="30">
+    <row r="28" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4" t="s">
         <v>88</v>
@@ -3449,7 +3455,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="6" customFormat="1" ht="45">
+    <row r="29" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4" t="s">
         <v>95</v>
@@ -3460,7 +3466,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="6" customFormat="1" ht="45">
+    <row r="30" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>37</v>
       </c>
@@ -3475,7 +3481,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="6" customFormat="1" ht="45">
+    <row r="31" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4" t="s">
         <v>78</v>
@@ -3488,7 +3494,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="6" customFormat="1" ht="45">
+    <row r="32" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4" t="s">
         <v>77</v>
@@ -3501,7 +3507,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="6" customFormat="1" ht="45">
+    <row r="33" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
         <v>181</v>
@@ -3514,7 +3520,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="6" customFormat="1" ht="45">
+    <row r="34" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4" t="s">
         <v>76</v>
@@ -3527,7 +3533,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="6" customFormat="1">
+    <row r="35" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>126</v>
       </c>
@@ -3536,7 +3542,7 @@
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
     </row>
-    <row r="36" spans="1:5" s="6" customFormat="1" ht="60">
+    <row r="36" spans="1:5" s="6" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3" t="s">
         <v>11</v>
@@ -3549,7 +3555,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="6" customFormat="1" ht="60">
+    <row r="37" spans="1:5" s="6" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3" t="s">
         <v>54</v>
@@ -3562,7 +3568,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="6" customFormat="1" ht="60">
+    <row r="38" spans="1:5" s="6" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
         <v>55</v>
@@ -3575,7 +3581,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="6" customFormat="1" ht="60">
+    <row r="39" spans="1:5" s="6" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3" t="s">
         <v>56</v>
@@ -3588,7 +3594,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="6" customFormat="1" ht="60">
+    <row r="40" spans="1:5" s="6" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3" t="s">
         <v>1</v>
@@ -3601,7 +3607,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="6" customFormat="1">
+    <row r="41" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>19</v>
       </c>
@@ -3610,7 +3616,7 @@
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
     </row>
-    <row r="42" spans="1:5" s="6" customFormat="1" ht="30">
+    <row r="42" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
         <v>14</v>
       </c>
@@ -3621,7 +3627,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="6" customFormat="1" ht="30">
+    <row r="43" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
         <v>15</v>
       </c>
@@ -3632,7 +3638,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="6" customFormat="1" ht="75">
+    <row r="44" spans="1:5" s="6" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="5" t="s">
         <v>68</v>
@@ -3645,7 +3651,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="6" customFormat="1">
+    <row r="45" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>21</v>
       </c>
@@ -3654,7 +3660,7 @@
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
     </row>
-    <row r="46" spans="1:5" s="9" customFormat="1" ht="45">
+    <row r="46" spans="1:5" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B46" s="21" t="s">
         <v>46</v>
       </c>
@@ -3665,7 +3671,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="6" customFormat="1" ht="30">
+    <row r="47" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3" t="s">
         <v>91</v>
@@ -3678,7 +3684,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="6" customFormat="1" ht="45">
+    <row r="48" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3" t="s">
         <v>17</v>
@@ -3691,7 +3697,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="6" customFormat="1">
+    <row r="49" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>36</v>
       </c>
@@ -3700,7 +3706,7 @@
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
     </row>
-    <row r="50" spans="1:5" s="6" customFormat="1" ht="30">
+    <row r="50" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B50" s="6" t="s">
         <v>81</v>
       </c>
@@ -3708,7 +3714,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="6" customFormat="1" ht="30">
+    <row r="51" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
         <v>16</v>
       </c>
@@ -3719,7 +3725,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="6" customFormat="1">
+    <row r="52" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>73</v>
       </c>
@@ -3728,600 +3734,611 @@
       <c r="D52" s="8"/>
       <c r="E52" s="8"/>
     </row>
-    <row r="53" spans="1:5" s="6" customFormat="1" ht="45">
+    <row r="53" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C54" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E54" s="3" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B54" s="4" t="s">
+    <row r="55" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C55" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="E55" s="3" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A55" s="6" t="s">
+    <row r="56" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B56" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C56" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E55" s="9" t="s">
+      <c r="E56" s="9" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B56" s="4" t="s">
+    <row r="57" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="C57" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E56" s="6" t="s">
+      <c r="E57" s="6" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B57" s="3" t="s">
+    <row r="58" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B58" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C58" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="E58" s="3" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B58" s="3" t="s">
+    <row r="59" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B59" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C59" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="E59" s="3" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B59" s="6" t="s">
+    <row r="60" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B60" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C60" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="E60" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A60" s="6" t="s">
+    <row r="61" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B61" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C61" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E60" s="9" t="s">
+      <c r="E61" s="9" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="61" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="D61" s="5"/>
-      <c r="E61" s="9" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" s="6" customFormat="1" ht="45">
+    <row r="62" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
       <c r="B62" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C62" s="5"/>
+        <v>177</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>178</v>
+      </c>
       <c r="D62" s="5"/>
       <c r="E62" s="9" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" s="6" customFormat="1" ht="45">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="B63" s="5" t="s">
-        <v>179</v>
+        <v>145</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="9" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="A64" s="5" t="s">
-        <v>37</v>
-      </c>
+        <v>239</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A64" s="5"/>
       <c r="B64" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>86</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="9" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" s="6" customFormat="1" ht="30">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="9" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D66" s="5"/>
+      <c r="E66" s="9" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="66" spans="1:5" s="6" customFormat="1">
-      <c r="A66" s="7" t="s">
+    <row r="67" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B66" s="8"/>
-      <c r="C66" s="8"/>
-      <c r="D66" s="8"/>
-      <c r="E66" s="8"/>
-    </row>
-    <row r="67" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="8"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="8"/>
+    </row>
+    <row r="68" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C67" s="6" t="s">
+      <c r="C68" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E67" s="3" t="s">
+      <c r="E68" s="3" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="68" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B68" s="4" t="s">
+    <row r="69" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C68" s="6" t="s">
+      <c r="C69" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="E69" s="3" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="69" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B69" s="4" t="s">
+    <row r="70" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B70" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C69" s="6" t="s">
+      <c r="C70" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E69" s="3" t="s">
+      <c r="E70" s="3" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="70" spans="1:5" s="6" customFormat="1" ht="105">
-      <c r="A70" s="5"/>
-      <c r="B70" s="5" t="s">
+    <row r="71" spans="1:5" s="6" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A71" s="5"/>
+      <c r="B71" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C71" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5" t="s">
+      <c r="D71" s="5"/>
+      <c r="E71" s="5" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="71" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="A71" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" s="6" customFormat="1" ht="30">
+    <row r="72" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B73" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="C72" s="6" t="s">
+      <c r="C73" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="E72" s="9" t="s">
+      <c r="E73" s="9" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="73" spans="1:5" s="6" customFormat="1">
-      <c r="A73" s="7" t="s">
+    <row r="74" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B73" s="8"/>
-      <c r="C73" s="8"/>
-      <c r="D73" s="8"/>
-      <c r="E73" s="8"/>
-    </row>
-    <row r="74" spans="1:5" s="12" customFormat="1" ht="45">
-      <c r="A74" s="5"/>
-      <c r="B74" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" s="12" customFormat="1" ht="30">
+      <c r="B74" s="8"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8"/>
+      <c r="E74" s="8"/>
+    </row>
+    <row r="75" spans="1:5" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="B75" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
       <c r="E75" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" s="12" customFormat="1" ht="30">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
       <c r="B76" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
       <c r="E76" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" s="12" customFormat="1" ht="45">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
       <c r="B77" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
       <c r="E77" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" s="12" customFormat="1" ht="30">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
       <c r="B78" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" s="6" customFormat="1" ht="45">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
       <c r="B79" s="20" t="s">
-        <v>96</v>
+        <v>171</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" s="6" customFormat="1" ht="45">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
       <c r="B80" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
       <c r="E80" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" s="6" customFormat="1" ht="30">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
-      <c r="B81" s="5" t="s">
-        <v>70</v>
+      <c r="B81" s="20" t="s">
+        <v>97</v>
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
       <c r="E81" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A82" s="5"/>
+      <c r="B82" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="4" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="82" spans="1:5" s="6" customFormat="1">
-      <c r="A82" s="7" t="s">
+    <row r="83" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B82" s="8"/>
-      <c r="C82" s="8"/>
-      <c r="D82" s="8"/>
-      <c r="E82" s="8"/>
-    </row>
-    <row r="83" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B83" s="6" t="s">
+      <c r="B83" s="8"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="8"/>
+      <c r="E83" s="8"/>
+    </row>
+    <row r="84" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B84" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="C83" s="6" t="s">
+      <c r="C84" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="E83" s="3" t="s">
+      <c r="E84" s="3" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="84" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B84" s="4" t="s">
+    <row r="85" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B85" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="C84" s="6" t="s">
+      <c r="C85" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="E84" s="3" t="s">
+      <c r="E85" s="3" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="85" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B85" s="6" t="s">
+    <row r="86" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B86" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="C85" s="6" t="s">
+      <c r="C86" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="E85" s="3" t="s">
+      <c r="E86" s="3" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="86" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B86" s="6" t="s">
+    <row r="87" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B87" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="C86" s="6" t="s">
+      <c r="C87" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="E86" s="3" t="s">
+      <c r="E87" s="3" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="87" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B87" s="6" t="s">
+    <row r="88" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B88" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="E87" s="3" t="s">
+      <c r="E88" s="3" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="88" spans="1:5" s="6" customFormat="1" ht="60">
-      <c r="B88" s="6" t="s">
+    <row r="89" spans="1:5" s="6" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="B89" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="E88" s="3" t="s">
+      <c r="E89" s="3" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="89" spans="1:5" s="6" customFormat="1" ht="60">
-      <c r="B89" s="6" t="s">
+    <row r="90" spans="1:5" s="6" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="B90" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="E89" s="3" t="s">
+      <c r="E90" s="3" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="90" spans="1:5" s="6" customFormat="1" ht="60">
-      <c r="B90" s="6" t="s">
+    <row r="91" spans="1:5" s="6" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="B91" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="E90" s="3" t="s">
+      <c r="E91" s="3" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="91" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B91" s="6" t="s">
+    <row r="92" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B92" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C91" s="6" t="s">
+      <c r="C92" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="E91" s="3" t="s">
+      <c r="E92" s="3" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="92" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B92" s="6" t="s">
+    <row r="93" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B93" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="C92" s="6" t="s">
+      <c r="C93" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="E92" s="3" t="s">
+      <c r="E93" s="3" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="93" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B93" s="6" t="s">
+    <row r="94" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B94" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="E93" s="3" t="s">
+      <c r="E94" s="3" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="94" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B94" s="6" t="s">
+    <row r="95" spans="1:5" s="6" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="B95" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="E94" s="3" t="s">
+      <c r="E95" s="3" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="95" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B95" s="6" t="s">
+    <row r="96" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B96" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="E95" s="3" t="s">
+      <c r="E96" s="3" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="96" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B96" s="6" t="s">
+    <row r="97" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B97" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="E96" s="3" t="s">
+      <c r="E97" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="97" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B97" s="4" t="s">
+    <row r="98" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B98" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="E97" s="3" t="s">
+      <c r="E98" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="98" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B98" s="4" t="s">
+    <row r="99" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B99" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="E98" s="3" t="s">
+      <c r="E99" s="3" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="99" spans="1:5" s="6" customFormat="1">
-      <c r="A99" s="7" t="s">
+    <row r="100" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="B99" s="8"/>
-      <c r="C99" s="8"/>
-      <c r="D99" s="8"/>
-      <c r="E99" s="8"/>
-    </row>
-    <row r="100" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B100" s="6" t="s">
+      <c r="B100" s="8"/>
+      <c r="C100" s="8"/>
+      <c r="D100" s="8"/>
+      <c r="E100" s="8"/>
+    </row>
+    <row r="101" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B101" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="E100" s="3" t="s">
+      <c r="E101" s="3" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="101" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B101" s="4" t="s">
+    <row r="102" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B102" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="E101" s="3" t="s">
+      <c r="E102" s="3" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="30">
-      <c r="A102" s="2" t="s">
+    <row r="103" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B102" s="18"/>
-      <c r="C102" s="18"/>
-      <c r="D102" s="14"/>
-      <c r="E102" s="19"/>
-    </row>
-    <row r="103" spans="1:5" s="15" customFormat="1" ht="30">
-      <c r="B103" s="15" t="s">
+      <c r="B103" s="18"/>
+      <c r="C103" s="18"/>
+      <c r="D103" s="14"/>
+      <c r="E103" s="19"/>
+    </row>
+    <row r="104" spans="1:5" s="15" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B104" s="15" t="s">
         <v>146</v>
-      </c>
-      <c r="D103" s="16"/>
-      <c r="E103" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" s="15" customFormat="1" ht="45">
-      <c r="B104" s="15" t="s">
-        <v>147</v>
       </c>
       <c r="D104" s="16"/>
       <c r="E104" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" s="15" customFormat="1" ht="45">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" s="15" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B105" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D105" s="16"/>
       <c r="E105" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" s="15" customFormat="1" ht="45">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" s="15" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B106" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D106" s="16"/>
       <c r="E106" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" s="15" customFormat="1" ht="45">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" s="15" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B107" s="15" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D107" s="16"/>
       <c r="E107" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" s="15" customFormat="1" ht="45">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" s="15" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B108" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D108" s="16"/>
       <c r="E108" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" s="15" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B109" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="D109" s="16"/>
+      <c r="E109" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="109" spans="1:5" s="6" customFormat="1">
-      <c r="E109" s="9"/>
-    </row>
-    <row r="110" spans="1:5" s="6" customFormat="1"/>
-    <row r="111" spans="1:5" s="6" customFormat="1"/>
-    <row r="112" spans="1:5" s="6" customFormat="1"/>
-    <row r="113" s="6" customFormat="1"/>
-    <row r="114" s="6" customFormat="1"/>
-    <row r="115" s="6" customFormat="1"/>
-    <row r="116" s="6" customFormat="1"/>
-    <row r="117" s="6" customFormat="1"/>
-    <row r="118" s="6" customFormat="1"/>
+    <row r="110" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E110" s="9"/>
+    </row>
+    <row r="111" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="113" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="114" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="115" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="116" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="117" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="118" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="119" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Minor tweaks to mapping spreadsheets.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReport.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="1185" windowWidth="17595" windowHeight="8505" tabRatio="500"/>
+    <workbookView xWindow="1050" yWindow="-15" windowWidth="17595" windowHeight="8505" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Booking Report" sheetId="1" r:id="rId1"/>
@@ -1871,10 +1871,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3117,8 +3117,8 @@
   <dimension ref="A1:E120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A46" sqref="A46:XFD46"/>
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E105" sqref="E105:E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3131,10 +3131,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="24"/>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
@@ -3670,7 +3670,7 @@
       <c r="E45" s="8"/>
     </row>
     <row r="46" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A46" s="24"/>
+      <c r="A46" s="23"/>
       <c r="B46" s="4" t="s">
         <v>251</v>
       </c>

</xml_diff>

<commit_message>
Added Offense (Date, Description, Category) to the Booking and Custody Status Change SSPs.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReport.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReport.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="-15" windowWidth="17595" windowHeight="8505" tabRatio="500"/>
+    <workbookView xWindow="-26780" yWindow="7140" windowWidth="29260" windowHeight="16460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Booking Report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="264">
   <si>
     <t>Race</t>
   </si>
@@ -781,6 +781,36 @@
   </si>
   <si>
     <t>/br-doc:BookingReport/j:Booking[@structures:id=/br-doc:BookingReport/j:ActivityCaseAssociation/nc:Activity/@structures:ref]/j:BookingAgencyRecordIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>Offense</t>
+  </si>
+  <si>
+    <t>Offense Description</t>
+  </si>
+  <si>
+    <t>Offense Category</t>
+  </si>
+  <si>
+    <t>Offense Date</t>
+  </si>
+  <si>
+    <t>The date of an offense</t>
+  </si>
+  <si>
+    <t>The description of an offense</t>
+  </si>
+  <si>
+    <t>A type of offense</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Offense[@structures:id=/br-doc:BookingReport/j:OffenseChargeAssociation/j:Offense/@structures:ref]/nc:ActivityDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Offense[@structures:id=/br-doc:BookingReport/j:OffenseChargeAssociation/j:Offense/@structures:ref]/nc:ActivityDescriptionText</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Offense[@structures:id=/br-doc:BookingReport/j:OffenseChargeAssociation/j:Offense/@structures:ref]/j:OffenseCategoryText</t>
   </si>
 </sst>
 </file>
@@ -899,9 +929,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="902">
+  <cellStyleXfs count="908">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1878,7 +1914,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="902">
+  <cellStyles count="908">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2329,6 +2365,9 @@
     <cellStyle name="Followed Hyperlink" xfId="897" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="899" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="901" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="903" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="905" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="907" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2779,6 +2818,9 @@
     <cellStyle name="Hyperlink" xfId="896" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="898" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="900" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="902" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="904" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="906" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3114,23 +3156,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E120"/>
+  <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E105" sqref="E105:E110"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.375" style="17" customWidth="1"/>
-    <col min="2" max="2" width="27.625" style="17" customWidth="1"/>
-    <col min="3" max="4" width="28.375" style="17" customWidth="1"/>
-    <col min="5" max="5" width="92.375" style="17" customWidth="1"/>
-    <col min="6" max="16384" width="10.875" style="17"/>
+    <col min="1" max="1" width="20.33203125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" style="17" customWidth="1"/>
+    <col min="3" max="4" width="28.33203125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="92.33203125" style="17" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="36" customHeight="1">
       <c r="A1" s="24" t="s">
         <v>43</v>
       </c>
@@ -3139,7 +3181,7 @@
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
     </row>
-    <row r="2" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="36" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -3156,7 +3198,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
@@ -3165,7 +3207,7 @@
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
     </row>
-    <row r="4" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="6" customFormat="1" ht="31.5">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>7</v>
@@ -3178,7 +3220,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="6" customFormat="1">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
         <v>5</v>
@@ -3191,7 +3233,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="6" customFormat="1">
       <c r="A6" s="7" t="s">
         <v>45</v>
       </c>
@@ -3200,7 +3242,7 @@
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="6" customFormat="1">
       <c r="A7" s="9"/>
       <c r="B7" s="9" t="s">
         <v>23</v>
@@ -3213,7 +3255,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="6" customFormat="1">
       <c r="A8" s="9"/>
       <c r="B8" s="9" t="s">
         <v>24</v>
@@ -3226,7 +3268,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="6" customFormat="1">
       <c r="A9" s="7" t="s">
         <v>97</v>
       </c>
@@ -3235,7 +3277,7 @@
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
         <v>98</v>
@@ -3246,7 +3288,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="6" customFormat="1">
       <c r="A11" s="7" t="s">
         <v>44</v>
       </c>
@@ -3255,7 +3297,7 @@
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
         <v>126</v>
@@ -3266,7 +3308,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
         <v>149</v>
@@ -3277,7 +3319,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="6" customFormat="1" ht="31.5">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
         <v>138</v>
@@ -3288,7 +3330,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" s="6" customFormat="1" ht="31.5">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
         <v>139</v>
@@ -3299,7 +3341,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
         <v>140</v>
@@ -3310,7 +3352,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
         <v>141</v>
@@ -3321,7 +3363,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
         <v>142</v>
@@ -3334,7 +3376,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
         <v>11</v>
@@ -3347,7 +3389,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" s="6" customFormat="1" ht="31.5">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
         <v>2</v>
@@ -3360,7 +3402,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" s="6" customFormat="1" ht="31.5">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
         <v>0</v>
@@ -3373,7 +3415,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
         <v>46</v>
@@ -3386,7 +3428,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
         <v>49</v>
@@ -3399,7 +3441,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
         <v>53</v>
@@ -3412,7 +3454,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
         <v>54</v>
@@ -3425,7 +3467,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
         <v>55</v>
@@ -3438,7 +3480,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" s="6" customFormat="1" ht="31.5">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
         <v>1</v>
@@ -3451,7 +3493,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" s="6" customFormat="1" ht="31.5">
       <c r="A28" s="4"/>
       <c r="B28" s="4" t="s">
         <v>87</v>
@@ -3464,7 +3506,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4" t="s">
         <v>94</v>
@@ -3475,7 +3517,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="A30" s="4" t="s">
         <v>37</v>
       </c>
@@ -3490,7 +3532,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4" t="s">
         <v>77</v>
@@ -3503,7 +3545,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4" t="s">
         <v>76</v>
@@ -3516,7 +3558,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
         <v>180</v>
@@ -3529,7 +3571,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4" t="s">
         <v>75</v>
@@ -3542,7 +3584,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" s="6" customFormat="1">
       <c r="A35" s="7" t="s">
         <v>125</v>
       </c>
@@ -3551,7 +3593,7 @@
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
     </row>
-    <row r="36" spans="1:5" s="6" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" s="6" customFormat="1" ht="63">
       <c r="A36" s="3"/>
       <c r="B36" s="3" t="s">
         <v>11</v>
@@ -3564,7 +3606,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="6" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" s="6" customFormat="1" ht="63">
       <c r="A37" s="3"/>
       <c r="B37" s="3" t="s">
         <v>53</v>
@@ -3577,7 +3619,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="6" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" s="6" customFormat="1" ht="63">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
         <v>54</v>
@@ -3590,7 +3632,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="6" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" s="6" customFormat="1" ht="63">
       <c r="A39" s="3"/>
       <c r="B39" s="3" t="s">
         <v>55</v>
@@ -3603,7 +3645,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="6" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" s="6" customFormat="1" ht="63">
       <c r="A40" s="3"/>
       <c r="B40" s="3" t="s">
         <v>1</v>
@@ -3616,7 +3658,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" s="6" customFormat="1">
       <c r="A41" s="7" t="s">
         <v>19</v>
       </c>
@@ -3625,7 +3667,7 @@
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
     </row>
-    <row r="42" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" s="6" customFormat="1" ht="31.5">
       <c r="B42" s="4" t="s">
         <v>14</v>
       </c>
@@ -3636,7 +3678,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" s="6" customFormat="1" ht="31.5">
       <c r="B43" s="4" t="s">
         <v>15</v>
       </c>
@@ -3647,7 +3689,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="6" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" s="6" customFormat="1" ht="78.75">
       <c r="A44" s="5"/>
       <c r="B44" s="5" t="s">
         <v>67</v>
@@ -3660,7 +3702,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" s="6" customFormat="1">
       <c r="A45" s="7" t="s">
         <v>21</v>
       </c>
@@ -3669,7 +3711,7 @@
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
     </row>
-    <row r="46" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="A46" s="23"/>
       <c r="B46" s="4" t="s">
         <v>251</v>
@@ -3680,7 +3722,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" s="9" customFormat="1" ht="47.25">
       <c r="B47" s="21" t="s">
         <v>252</v>
       </c>
@@ -3691,7 +3733,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" s="6" customFormat="1" ht="31.5">
       <c r="A48" s="3"/>
       <c r="B48" s="3" t="s">
         <v>90</v>
@@ -3704,7 +3746,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="A49" s="3"/>
       <c r="B49" s="3" t="s">
         <v>17</v>
@@ -3717,7 +3759,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" s="6" customFormat="1">
       <c r="A50" s="7" t="s">
         <v>36</v>
       </c>
@@ -3726,7 +3768,7 @@
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
     </row>
-    <row r="51" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" s="6" customFormat="1" ht="31.5">
       <c r="B51" s="6" t="s">
         <v>80</v>
       </c>
@@ -3734,7 +3776,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" s="6" customFormat="1" ht="31.5">
       <c r="B52" s="4" t="s">
         <v>16</v>
       </c>
@@ -3745,7 +3787,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" s="6" customFormat="1">
       <c r="A53" s="7" t="s">
         <v>72</v>
       </c>
@@ -3754,7 +3796,7 @@
       <c r="D53" s="8"/>
       <c r="E53" s="8"/>
     </row>
-    <row r="54" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="B54" s="4" t="s">
         <v>249</v>
       </c>
@@ -3765,7 +3807,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="B55" s="4" t="s">
         <v>92</v>
       </c>
@@ -3776,7 +3818,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" s="6" customFormat="1" ht="31.5">
       <c r="B56" s="4" t="s">
         <v>18</v>
       </c>
@@ -3787,7 +3829,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="A57" s="6" t="s">
         <v>37</v>
       </c>
@@ -3801,7 +3843,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="B58" s="4" t="s">
         <v>35</v>
       </c>
@@ -3812,7 +3854,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="B59" s="3" t="s">
         <v>56</v>
       </c>
@@ -3823,7 +3865,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="B60" s="3" t="s">
         <v>57</v>
       </c>
@@ -3834,7 +3876,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="61" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="B61" s="6" t="s">
         <v>58</v>
       </c>
@@ -3845,7 +3887,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="62" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="A62" s="6" t="s">
         <v>93</v>
       </c>
@@ -3859,7 +3901,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="A63" s="5"/>
       <c r="B63" s="5" t="s">
         <v>176</v>
@@ -3872,7 +3914,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="64" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="A64" s="5"/>
       <c r="B64" s="5" t="s">
         <v>144</v>
@@ -3883,7 +3925,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="A65" s="5"/>
       <c r="B65" s="5" t="s">
         <v>178</v>
@@ -3894,7 +3936,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="66" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" s="6" customFormat="1" ht="47.25">
       <c r="A66" s="5" t="s">
         <v>37</v>
       </c>
@@ -3909,7 +3951,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="67" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" s="6" customFormat="1" ht="31.5">
       <c r="A67" s="5" t="s">
         <v>37</v>
       </c>
@@ -3924,448 +3966,490 @@
         <v>241</v>
       </c>
     </row>
-    <row r="68" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" s="6" customFormat="1">
       <c r="A68" s="7" t="s">
-        <v>33</v>
+        <v>254</v>
       </c>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
       <c r="D68" s="8"/>
       <c r="E68" s="8"/>
     </row>
-    <row r="69" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="B69" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B70" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B71" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="6" customFormat="1">
+      <c r="A72" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B72" s="8"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+    </row>
+    <row r="73" spans="1:5" s="6" customFormat="1" ht="31.5">
+      <c r="B73" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C69" s="6" t="s">
+      <c r="C73" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E69" s="3" t="s">
+      <c r="E73" s="3" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="70" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B70" s="4" t="s">
+    <row r="74" spans="1:5" s="6" customFormat="1" ht="31.5">
+      <c r="B74" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C70" s="6" t="s">
+      <c r="C74" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E70" s="3" t="s">
+      <c r="E74" s="3" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="71" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B71" s="4" t="s">
+    <row r="75" spans="1:5" s="6" customFormat="1" ht="47.25">
+      <c r="B75" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C71" s="6" t="s">
+      <c r="C75" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E71" s="3" t="s">
+      <c r="E75" s="3" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="72" spans="1:5" s="6" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A72" s="5"/>
-      <c r="B72" s="5" t="s">
+    <row r="76" spans="1:5" s="6" customFormat="1" ht="110.25">
+      <c r="A76" s="5"/>
+      <c r="B76" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C72" s="5" t="s">
+      <c r="C76" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D72" s="5"/>
-      <c r="E72" s="5" t="s">
+      <c r="D76" s="5"/>
+      <c r="E76" s="5" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="73" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A73" s="6" t="s">
+    <row r="77" spans="1:5" s="6" customFormat="1" ht="31.5">
+      <c r="A77" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B73" s="6" t="s">
+      <c r="B77" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C73" s="6" t="s">
+      <c r="C77" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E73" s="3" t="s">
+      <c r="E77" s="3" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="74" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A74" s="6" t="s">
+    <row r="78" spans="1:5" s="6" customFormat="1" ht="31.5">
+      <c r="A78" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B78" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="C74" s="6" t="s">
+      <c r="C78" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="E74" s="9" t="s">
+      <c r="E78" s="9" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="7" t="s">
+    <row r="79" spans="1:5" s="6" customFormat="1">
+      <c r="A79" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B75" s="8"/>
-      <c r="C75" s="8"/>
-      <c r="D75" s="8"/>
-      <c r="E75" s="8"/>
-    </row>
-    <row r="76" spans="1:5" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A76" s="5"/>
-      <c r="B76" s="20" t="s">
-        <v>166</v>
-      </c>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
-      <c r="E76" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A77" s="5"/>
-      <c r="B77" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="5"/>
-      <c r="B78" s="20" t="s">
-        <v>168</v>
-      </c>
-      <c r="C78" s="5"/>
-      <c r="D78" s="5"/>
-      <c r="E78" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A79" s="5"/>
-      <c r="B79" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B79" s="8"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="8"/>
+      <c r="E79" s="8"/>
+    </row>
+    <row r="80" spans="1:5" s="12" customFormat="1" ht="47.25">
       <c r="A80" s="5"/>
       <c r="B80" s="20" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
       <c r="E80" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" s="12" customFormat="1" ht="31.5">
       <c r="A81" s="5"/>
       <c r="B81" s="20" t="s">
-        <v>95</v>
+        <v>167</v>
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
       <c r="E81" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" s="12" customFormat="1" ht="31.5">
       <c r="A82" s="5"/>
       <c r="B82" s="20" t="s">
-        <v>96</v>
+        <v>168</v>
       </c>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
       <c r="E82" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" s="12" customFormat="1" ht="47.25">
       <c r="A83" s="5"/>
-      <c r="B83" s="5" t="s">
-        <v>69</v>
+      <c r="B83" s="20" t="s">
+        <v>169</v>
       </c>
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
       <c r="E83" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" s="12" customFormat="1" ht="31.5">
+      <c r="A84" s="5"/>
+      <c r="B84" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" s="6" customFormat="1" ht="47.25">
+      <c r="A85" s="5"/>
+      <c r="B85" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
+      <c r="E85" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" s="6" customFormat="1" ht="47.25">
+      <c r="A86" s="5"/>
+      <c r="B86" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" s="6" customFormat="1" ht="31.5">
+      <c r="A87" s="5"/>
+      <c r="B87" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C87" s="5"/>
+      <c r="D87" s="5"/>
+      <c r="E87" s="4" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="84" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="7" t="s">
+    <row r="88" spans="1:5" s="6" customFormat="1">
+      <c r="A88" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="B84" s="8"/>
-      <c r="C84" s="8"/>
-      <c r="D84" s="8"/>
-      <c r="E84" s="8"/>
-    </row>
-    <row r="85" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B85" s="6" t="s">
+      <c r="B88" s="8"/>
+      <c r="C88" s="8"/>
+      <c r="D88" s="8"/>
+      <c r="E88" s="8"/>
+    </row>
+    <row r="89" spans="1:5" s="6" customFormat="1" ht="47.25">
+      <c r="B89" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="C85" s="6" t="s">
+      <c r="C89" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="E85" s="3" t="s">
+      <c r="E89" s="3" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="86" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B86" s="4" t="s">
+    <row r="90" spans="1:5" s="6" customFormat="1" ht="47.25">
+      <c r="B90" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="C86" s="6" t="s">
+      <c r="C90" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="E86" s="3" t="s">
+      <c r="E90" s="3" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="87" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B87" s="6" t="s">
+    <row r="91" spans="1:5" s="6" customFormat="1" ht="47.25">
+      <c r="B91" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="C87" s="6" t="s">
+      <c r="C91" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="E87" s="3" t="s">
+      <c r="E91" s="3" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="88" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B88" s="6" t="s">
+    <row r="92" spans="1:5" s="6" customFormat="1" ht="47.25">
+      <c r="B92" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="C88" s="6" t="s">
+      <c r="C92" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="E88" s="3" t="s">
+      <c r="E92" s="3" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="89" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B89" s="6" t="s">
+    <row r="93" spans="1:5" s="6" customFormat="1" ht="47.25">
+      <c r="B93" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="E89" s="3" t="s">
+      <c r="E93" s="3" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="90" spans="1:5" s="6" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="B90" s="6" t="s">
+    <row r="94" spans="1:5" s="6" customFormat="1" ht="63">
+      <c r="B94" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="E90" s="3" t="s">
+      <c r="E94" s="3" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="91" spans="1:5" s="6" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="B91" s="6" t="s">
+    <row r="95" spans="1:5" s="6" customFormat="1" ht="63">
+      <c r="B95" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="E91" s="3" t="s">
+      <c r="E95" s="3" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="92" spans="1:5" s="6" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="B92" s="6" t="s">
+    <row r="96" spans="1:5" s="6" customFormat="1" ht="63">
+      <c r="B96" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="E92" s="3" t="s">
+      <c r="E96" s="3" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="93" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B93" s="6" t="s">
+    <row r="97" spans="1:5" s="6" customFormat="1" ht="47.25">
+      <c r="B97" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="C93" s="6" t="s">
+      <c r="C97" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="E93" s="3" t="s">
+      <c r="E97" s="3" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="94" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B94" s="6" t="s">
+    <row r="98" spans="1:5" s="6" customFormat="1" ht="47.25">
+      <c r="B98" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="C94" s="6" t="s">
+      <c r="C98" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="E94" s="3" t="s">
+      <c r="E98" s="3" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="95" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B95" s="6" t="s">
+    <row r="99" spans="1:5" s="6" customFormat="1" ht="47.25">
+      <c r="B99" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="E95" s="3" t="s">
+      <c r="E99" s="3" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="96" spans="1:5" s="6" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="B96" s="6" t="s">
+    <row r="100" spans="1:5" s="6" customFormat="1" ht="63">
+      <c r="B100" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="E96" s="3" t="s">
+      <c r="E100" s="3" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="97" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B97" s="6" t="s">
+    <row r="101" spans="1:5" s="6" customFormat="1" ht="47.25">
+      <c r="B101" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="E97" s="3" t="s">
+      <c r="E101" s="3" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="98" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B98" s="6" t="s">
+    <row r="102" spans="1:5" s="6" customFormat="1" ht="47.25">
+      <c r="B102" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="E98" s="3" t="s">
+      <c r="E102" s="3" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="99" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B99" s="4" t="s">
+    <row r="103" spans="1:5" s="6" customFormat="1" ht="47.25">
+      <c r="B103" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="E99" s="3" t="s">
+      <c r="E103" s="3" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="100" spans="1:5" s="6" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B100" s="4" t="s">
+    <row r="104" spans="1:5" s="6" customFormat="1" ht="47.25">
+      <c r="B104" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="E100" s="3" t="s">
+      <c r="E104" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="101" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="7" t="s">
+    <row r="105" spans="1:5" s="6" customFormat="1">
+      <c r="A105" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="B101" s="8"/>
-      <c r="C101" s="8"/>
-      <c r="D101" s="8"/>
-      <c r="E101" s="8"/>
-    </row>
-    <row r="102" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B102" s="6" t="s">
+      <c r="B105" s="8"/>
+      <c r="C105" s="8"/>
+      <c r="D105" s="8"/>
+      <c r="E105" s="8"/>
+    </row>
+    <row r="106" spans="1:5" s="6" customFormat="1" ht="31.5">
+      <c r="B106" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="E102" s="3" t="s">
+      <c r="E106" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="103" spans="1:5" s="6" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B103" s="4" t="s">
+    <row r="107" spans="1:5" s="6" customFormat="1" ht="31.5">
+      <c r="B107" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="E103" s="3" t="s">
+      <c r="E107" s="3" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
+    <row r="108" spans="1:5" ht="31.5">
+      <c r="A108" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B104" s="18"/>
-      <c r="C104" s="18"/>
-      <c r="D104" s="14"/>
-      <c r="E104" s="19"/>
-    </row>
-    <row r="105" spans="1:5" s="15" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B105" s="15" t="s">
+      <c r="B108" s="18"/>
+      <c r="C108" s="18"/>
+      <c r="D108" s="14"/>
+      <c r="E108" s="19"/>
+    </row>
+    <row r="109" spans="1:5" s="15" customFormat="1" ht="47.25">
+      <c r="B109" s="15" t="s">
         <v>145</v>
-      </c>
-      <c r="D105" s="16"/>
-      <c r="E105" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" s="15" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B106" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="D106" s="16"/>
-      <c r="E106" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" s="15" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B107" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="D107" s="16"/>
-      <c r="E107" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" s="15" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B108" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="D108" s="16"/>
-      <c r="E108" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" s="15" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B109" s="15" t="s">
-        <v>152</v>
       </c>
       <c r="D109" s="16"/>
       <c r="E109" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" s="15" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" s="15" customFormat="1" ht="47.25">
       <c r="B110" s="15" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D110" s="16"/>
       <c r="E110" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" s="15" customFormat="1" ht="47.25">
+      <c r="B111" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="D111" s="16"/>
+      <c r="E111" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" s="15" customFormat="1" ht="47.25">
+      <c r="B112" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="D112" s="16"/>
+      <c r="E112" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" s="15" customFormat="1" ht="47.25">
+      <c r="B113" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="D113" s="16"/>
+      <c r="E113" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" s="15" customFormat="1" ht="47.25">
+      <c r="B114" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D114" s="16"/>
+      <c r="E114" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="111" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E111" s="9"/>
-    </row>
-    <row r="112" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="113" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="114" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="115" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="116" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="117" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="118" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="119" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="120" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="115" spans="2:5" s="6" customFormat="1">
+      <c r="E115" s="9"/>
+    </row>
+    <row r="116" spans="2:5" s="6" customFormat="1"/>
+    <row r="117" spans="2:5" s="6" customFormat="1"/>
+    <row r="118" spans="2:5" s="6" customFormat="1"/>
+    <row r="119" spans="2:5" s="6" customFormat="1"/>
+    <row r="120" spans="2:5" s="6" customFormat="1"/>
+    <row r="121" spans="2:5" s="6" customFormat="1"/>
+    <row r="122" spans="2:5" s="6" customFormat="1"/>
+    <row r="123" spans="2:5" s="6" customFormat="1"/>
+    <row r="124" spans="2:5" s="6" customFormat="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added "PersonRaceCode" for Adams County to the 3 SSPs.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReport.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-26780" yWindow="7140" windowWidth="29260" windowHeight="16460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Booking Report" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="266">
   <si>
     <t>Race</t>
   </si>
@@ -811,6 +811,12 @@
   </si>
   <si>
     <t>/br-doc:BookingReport/j:Offense[@structures:id=/br-doc:BookingReport/j:OffenseChargeAssociation/j:Offense/@structures:ref]/j:OffenseCategoryText</t>
+  </si>
+  <si>
+    <t>Race Code (Adams County)</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/ac-bkg-codes:PersonRaceCode</t>
   </si>
 </sst>
 </file>
@@ -929,9 +935,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="908">
+  <cellStyleXfs count="916">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1914,7 +1928,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="908">
+  <cellStyles count="916">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2368,6 +2382,10 @@
     <cellStyle name="Followed Hyperlink" xfId="903" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="905" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="907" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="909" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="911" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="913" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="915" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2821,6 +2839,10 @@
     <cellStyle name="Hyperlink" xfId="902" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="904" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="906" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="908" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="910" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="912" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="914" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3156,11 +3178,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E124"/>
+  <dimension ref="A1:E125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D73" sqref="D73"/>
+      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3207,7 +3229,7 @@
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
     </row>
-    <row r="4" spans="1:5" s="6" customFormat="1" ht="31.5">
+    <row r="4" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>7</v>
@@ -3277,7 +3299,7 @@
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:5" s="6" customFormat="1" ht="47.25">
+    <row r="10" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
         <v>98</v>
@@ -3297,7 +3319,7 @@
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:5" s="6" customFormat="1" ht="47.25">
+    <row r="12" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
         <v>126</v>
@@ -3308,7 +3330,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="6" customFormat="1" ht="47.25">
+    <row r="13" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
         <v>149</v>
@@ -3319,7 +3341,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="6" customFormat="1" ht="31.5">
+    <row r="14" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
         <v>138</v>
@@ -3330,7 +3352,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="6" customFormat="1" ht="31.5">
+    <row r="15" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
         <v>139</v>
@@ -3341,7 +3363,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="6" customFormat="1" ht="47.25">
+    <row r="16" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
         <v>140</v>
@@ -3352,7 +3374,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="6" customFormat="1" ht="47.25">
+    <row r="17" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
         <v>141</v>
@@ -3363,7 +3385,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="6" customFormat="1" ht="47.25">
+    <row r="18" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
         <v>142</v>
@@ -3376,7 +3398,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="6" customFormat="1" ht="47.25">
+    <row r="19" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
         <v>11</v>
@@ -3389,7 +3411,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="6" customFormat="1" ht="31.5">
+    <row r="20" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
         <v>2</v>
@@ -3402,7 +3424,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="6" customFormat="1" ht="31.5">
+    <row r="21" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
         <v>0</v>
@@ -3415,1026 +3437,1039 @@
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="6" customFormat="1" ht="47.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3" t="s">
-        <v>46</v>
+    <row r="22" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A22" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>264</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="6" customFormat="1" ht="47.25">
+        <v>29</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="6" customFormat="1" ht="47.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="6" customFormat="1" ht="47.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="6" customFormat="1" ht="47.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" s="6" customFormat="1" ht="31.5">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3" t="s">
+      <c r="D28" s="3"/>
+      <c r="E28" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="6" customFormat="1" ht="31.5">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" s="6" customFormat="1" ht="47.25">
+    <row r="29" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A29" s="4"/>
       <c r="B29" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="11"/>
+      <c r="E29" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="6" customFormat="1" ht="47.25">
-      <c r="A30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>81</v>
-      </c>
+      <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="6" customFormat="1" ht="47.25">
-      <c r="A31" s="4"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A31" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="B31" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" s="6" customFormat="1" ht="47.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A32" s="4"/>
       <c r="B32" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="6" customFormat="1" ht="47.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
-        <v>180</v>
+        <v>76</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>181</v>
+        <v>82</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="6" customFormat="1" ht="47.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A34" s="4"/>
       <c r="B34" s="4" t="s">
-        <v>75</v>
+        <v>180</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>84</v>
+        <v>181</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="6" customFormat="1">
-      <c r="A35" s="7" t="s">
+    <row r="36" spans="1:5" s="6" customFormat="1">
+      <c r="A36" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-    </row>
-    <row r="36" spans="1:5" s="6" customFormat="1" ht="63">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D36" s="3"/>
-      <c r="E36" s="22" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="6" customFormat="1" ht="63">
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+    </row>
+    <row r="37" spans="1:5" s="6" customFormat="1" ht="60">
       <c r="A37" s="3"/>
       <c r="B37" s="3" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="22" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="6" customFormat="1" ht="63">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="6" customFormat="1" ht="60">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="22" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="6" customFormat="1" ht="63">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="6" customFormat="1" ht="60">
       <c r="A39" s="3"/>
       <c r="B39" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="22" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" s="6" customFormat="1" ht="63">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="6" customFormat="1" ht="60">
       <c r="A40" s="3"/>
       <c r="B40" s="3" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>129</v>
+        <v>52</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="22" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="6" customFormat="1" ht="60">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="22" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="6" customFormat="1">
-      <c r="A41" s="7" t="s">
+    <row r="42" spans="1:5" s="6" customFormat="1">
+      <c r="A42" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-    </row>
-    <row r="42" spans="1:5" s="6" customFormat="1" ht="31.5">
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+    </row>
+    <row r="43" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B43" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C43" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E43" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="6" customFormat="1" ht="31.5">
-      <c r="B43" s="4" t="s">
+    <row r="44" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B44" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C44" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E44" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="6" customFormat="1" ht="78.75">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5" t="s">
+    <row r="45" spans="1:5" s="6" customFormat="1" ht="75">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C45" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D44" s="5"/>
-      <c r="E44" s="3" t="s">
+      <c r="D45" s="5"/>
+      <c r="E45" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="6" customFormat="1">
-      <c r="A45" s="7" t="s">
+    <row r="46" spans="1:5" s="6" customFormat="1">
+      <c r="A46" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-    </row>
-    <row r="46" spans="1:5" s="6" customFormat="1" ht="47.25">
-      <c r="A46" s="23"/>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+    </row>
+    <row r="47" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A47" s="23"/>
+      <c r="B47" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="6" t="s">
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="6" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="9" customFormat="1" ht="47.25">
-      <c r="B47" s="21" t="s">
+    <row r="48" spans="1:5" s="9" customFormat="1" ht="45">
+      <c r="B48" s="21" t="s">
         <v>252</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="C48" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E47" s="6" t="s">
+      <c r="E48" s="6" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="6" customFormat="1" ht="31.5">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" s="6" customFormat="1" ht="47.25">
+    <row r="49" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A49" s="3"/>
       <c r="B49" s="3" t="s">
-        <v>17</v>
+        <v>90</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="6" customFormat="1">
-      <c r="A50" s="7" t="s">
+    <row r="51" spans="1:5" s="6" customFormat="1">
+      <c r="A51" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-    </row>
-    <row r="51" spans="1:5" s="6" customFormat="1" ht="31.5">
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+    </row>
+    <row r="52" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B52" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="E52" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="6" customFormat="1" ht="31.5">
-      <c r="B52" s="4" t="s">
+    <row r="53" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B53" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C52" s="6" t="s">
+      <c r="C53" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E53" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="6" customFormat="1">
-      <c r="A53" s="7" t="s">
+    <row r="54" spans="1:5" s="6" customFormat="1">
+      <c r="A54" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="8"/>
-    </row>
-    <row r="54" spans="1:5" s="6" customFormat="1" ht="47.25">
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+    </row>
+    <row r="55" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B55" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C55" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="E55" s="3" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="6" customFormat="1" ht="47.25">
-      <c r="B55" s="4" t="s">
+    <row r="56" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B56" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C56" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E56" s="3" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="6" customFormat="1" ht="31.5">
-      <c r="B56" s="4" t="s">
+    <row r="57" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B57" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="C57" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E57" s="3" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="6" customFormat="1" ht="47.25">
-      <c r="A57" s="6" t="s">
+    <row r="58" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A58" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B58" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C58" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E57" s="9" t="s">
+      <c r="E58" s="9" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="6" customFormat="1" ht="47.25">
-      <c r="B58" s="4" t="s">
+    <row r="59" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B59" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C59" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E58" s="6" t="s">
+      <c r="E59" s="6" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="6" customFormat="1" ht="47.25">
-      <c r="B59" s="3" t="s">
+    <row r="60" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B60" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C60" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="E60" s="3" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="6" customFormat="1" ht="47.25">
-      <c r="B60" s="3" t="s">
+    <row r="61" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B61" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C61" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="E61" s="3" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="61" spans="1:5" s="6" customFormat="1" ht="47.25">
-      <c r="B61" s="6" t="s">
+    <row r="62" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B62" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C62" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E62" s="3" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="62" spans="1:5" s="6" customFormat="1" ht="47.25">
-      <c r="A62" s="6" t="s">
+    <row r="63" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A63" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="B63" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C63" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E62" s="9" t="s">
+      <c r="E63" s="9" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="6" customFormat="1" ht="47.25">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="D63" s="5"/>
-      <c r="E63" s="9" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" s="6" customFormat="1" ht="47.25">
+    <row r="64" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A64" s="5"/>
       <c r="B64" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C64" s="5"/>
+        <v>176</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>177</v>
+      </c>
       <c r="D64" s="5"/>
       <c r="E64" s="9" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" s="6" customFormat="1" ht="47.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A65" s="5"/>
       <c r="B65" s="5" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="9" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" s="6" customFormat="1" ht="47.25">
-      <c r="A66" s="5" t="s">
-        <v>37</v>
-      </c>
+        <v>238</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A66" s="5"/>
       <c r="B66" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>85</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="9" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" s="6" customFormat="1" ht="31.5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A67" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="9" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="A68" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D68" s="5"/>
+      <c r="E68" s="9" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="68" spans="1:5" s="6" customFormat="1">
-      <c r="A68" s="7" t="s">
+    <row r="69" spans="1:5" s="6" customFormat="1">
+      <c r="A69" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="B68" s="8"/>
-      <c r="C68" s="8"/>
-      <c r="D68" s="8"/>
-      <c r="E68" s="8"/>
-    </row>
-    <row r="69" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B69" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>261</v>
-      </c>
+      <c r="B69" s="8"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="8"/>
     </row>
     <row r="70" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="B70" s="4" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="71" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="B71" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B72" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="C71" s="6" t="s">
+      <c r="C72" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="E71" s="3" t="s">
+      <c r="E72" s="3" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="72" spans="1:5" s="6" customFormat="1">
-      <c r="A72" s="7" t="s">
+    <row r="73" spans="1:5" s="6" customFormat="1">
+      <c r="A73" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B72" s="8"/>
-      <c r="C72" s="8"/>
-      <c r="D72" s="8"/>
-      <c r="E72" s="8"/>
-    </row>
-    <row r="73" spans="1:5" s="6" customFormat="1" ht="31.5">
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="8"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="8"/>
+      <c r="E73" s="8"/>
+    </row>
+    <row r="74" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B74" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C73" s="6" t="s">
+      <c r="C74" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E73" s="3" t="s">
+      <c r="E74" s="3" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="74" spans="1:5" s="6" customFormat="1" ht="31.5">
-      <c r="B74" s="4" t="s">
+    <row r="75" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B75" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C74" s="6" t="s">
+      <c r="C75" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E74" s="3" t="s">
+      <c r="E75" s="3" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="6" customFormat="1" ht="47.25">
-      <c r="B75" s="4" t="s">
+    <row r="76" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B76" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C75" s="6" t="s">
+      <c r="C76" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E75" s="3" t="s">
+      <c r="E76" s="3" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="76" spans="1:5" s="6" customFormat="1" ht="110.25">
-      <c r="A76" s="5"/>
-      <c r="B76" s="5" t="s">
+    <row r="77" spans="1:5" s="6" customFormat="1" ht="105">
+      <c r="A77" s="5"/>
+      <c r="B77" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="C77" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5" t="s">
+      <c r="D77" s="5"/>
+      <c r="E77" s="5" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="77" spans="1:5" s="6" customFormat="1" ht="31.5">
-      <c r="A77" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" s="6" customFormat="1" ht="31.5">
+    <row r="78" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A78" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B78" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="A79" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B79" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="C78" s="6" t="s">
+      <c r="C79" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="E78" s="9" t="s">
+      <c r="E79" s="9" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="79" spans="1:5" s="6" customFormat="1">
-      <c r="A79" s="7" t="s">
+    <row r="80" spans="1:5" s="6" customFormat="1">
+      <c r="A80" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B79" s="8"/>
-      <c r="C79" s="8"/>
-      <c r="D79" s="8"/>
-      <c r="E79" s="8"/>
-    </row>
-    <row r="80" spans="1:5" s="12" customFormat="1" ht="47.25">
-      <c r="A80" s="5"/>
-      <c r="B80" s="20" t="s">
-        <v>166</v>
-      </c>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
-      <c r="E80" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" s="12" customFormat="1" ht="31.5">
+      <c r="B80" s="8"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+      <c r="E80" s="8"/>
+    </row>
+    <row r="81" spans="1:5" s="12" customFormat="1" ht="45">
       <c r="A81" s="5"/>
       <c r="B81" s="20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
       <c r="E81" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" s="12" customFormat="1" ht="31.5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" s="12" customFormat="1" ht="30">
       <c r="A82" s="5"/>
       <c r="B82" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
       <c r="E82" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" s="12" customFormat="1" ht="47.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" s="12" customFormat="1" ht="30">
       <c r="A83" s="5"/>
       <c r="B83" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
       <c r="E83" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" s="12" customFormat="1" ht="31.5">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" s="12" customFormat="1" ht="45">
       <c r="A84" s="5"/>
       <c r="B84" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
       <c r="E84" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" s="6" customFormat="1" ht="47.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" s="12" customFormat="1" ht="30">
       <c r="A85" s="5"/>
       <c r="B85" s="20" t="s">
-        <v>95</v>
+        <v>170</v>
       </c>
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
       <c r="E85" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" s="6" customFormat="1" ht="47.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A86" s="5"/>
       <c r="B86" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
       <c r="E86" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" s="6" customFormat="1" ht="31.5">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A87" s="5"/>
-      <c r="B87" s="5" t="s">
-        <v>69</v>
+      <c r="B87" s="20" t="s">
+        <v>96</v>
       </c>
       <c r="C87" s="5"/>
       <c r="D87" s="5"/>
       <c r="E87" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="A88" s="5"/>
+      <c r="B88" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C88" s="5"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="4" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="88" spans="1:5" s="6" customFormat="1">
-      <c r="A88" s="7" t="s">
+    <row r="89" spans="1:5" s="6" customFormat="1">
+      <c r="A89" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="B88" s="8"/>
-      <c r="C88" s="8"/>
-      <c r="D88" s="8"/>
-      <c r="E88" s="8"/>
-    </row>
-    <row r="89" spans="1:5" s="6" customFormat="1" ht="47.25">
-      <c r="B89" s="6" t="s">
+      <c r="B89" s="8"/>
+      <c r="C89" s="8"/>
+      <c r="D89" s="8"/>
+      <c r="E89" s="8"/>
+    </row>
+    <row r="90" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B90" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="C89" s="6" t="s">
+      <c r="C90" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="E89" s="3" t="s">
+      <c r="E90" s="3" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="90" spans="1:5" s="6" customFormat="1" ht="47.25">
-      <c r="B90" s="4" t="s">
+    <row r="91" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B91" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="C90" s="6" t="s">
+      <c r="C91" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="E90" s="3" t="s">
+      <c r="E91" s="3" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="91" spans="1:5" s="6" customFormat="1" ht="47.25">
-      <c r="B91" s="6" t="s">
+    <row r="92" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B92" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="C91" s="6" t="s">
+      <c r="C92" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="E91" s="3" t="s">
+      <c r="E92" s="3" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="92" spans="1:5" s="6" customFormat="1" ht="47.25">
-      <c r="B92" s="6" t="s">
+    <row r="93" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B93" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="C92" s="6" t="s">
+      <c r="C93" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="E92" s="3" t="s">
+      <c r="E93" s="3" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="93" spans="1:5" s="6" customFormat="1" ht="47.25">
-      <c r="B93" s="6" t="s">
+    <row r="94" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B94" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="E93" s="3" t="s">
+      <c r="E94" s="3" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="94" spans="1:5" s="6" customFormat="1" ht="63">
-      <c r="B94" s="6" t="s">
+    <row r="95" spans="1:5" s="6" customFormat="1" ht="60">
+      <c r="B95" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="E94" s="3" t="s">
+      <c r="E95" s="3" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="95" spans="1:5" s="6" customFormat="1" ht="63">
-      <c r="B95" s="6" t="s">
+    <row r="96" spans="1:5" s="6" customFormat="1" ht="60">
+      <c r="B96" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="E95" s="3" t="s">
+      <c r="E96" s="3" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="96" spans="1:5" s="6" customFormat="1" ht="63">
-      <c r="B96" s="6" t="s">
+    <row r="97" spans="1:5" s="6" customFormat="1" ht="60">
+      <c r="B97" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="E96" s="3" t="s">
+      <c r="E97" s="3" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="97" spans="1:5" s="6" customFormat="1" ht="47.25">
-      <c r="B97" s="6" t="s">
+    <row r="98" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B98" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="C97" s="6" t="s">
+      <c r="C98" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="E97" s="3" t="s">
+      <c r="E98" s="3" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="98" spans="1:5" s="6" customFormat="1" ht="47.25">
-      <c r="B98" s="6" t="s">
+    <row r="99" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B99" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="C98" s="6" t="s">
+      <c r="C99" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="E98" s="3" t="s">
+      <c r="E99" s="3" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="99" spans="1:5" s="6" customFormat="1" ht="47.25">
-      <c r="B99" s="6" t="s">
+    <row r="100" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B100" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="E99" s="3" t="s">
+      <c r="E100" s="3" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="100" spans="1:5" s="6" customFormat="1" ht="63">
-      <c r="B100" s="6" t="s">
+    <row r="101" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B101" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="E100" s="3" t="s">
+      <c r="E101" s="3" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="101" spans="1:5" s="6" customFormat="1" ht="47.25">
-      <c r="B101" s="6" t="s">
+    <row r="102" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B102" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="E101" s="3" t="s">
+      <c r="E102" s="3" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="102" spans="1:5" s="6" customFormat="1" ht="47.25">
-      <c r="B102" s="6" t="s">
+    <row r="103" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B103" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="E102" s="3" t="s">
+      <c r="E103" s="3" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="103" spans="1:5" s="6" customFormat="1" ht="47.25">
-      <c r="B103" s="4" t="s">
+    <row r="104" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B104" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="E103" s="3" t="s">
+      <c r="E104" s="3" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="104" spans="1:5" s="6" customFormat="1" ht="47.25">
-      <c r="B104" s="4" t="s">
+    <row r="105" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B105" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="E104" s="3" t="s">
+      <c r="E105" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="105" spans="1:5" s="6" customFormat="1">
-      <c r="A105" s="7" t="s">
+    <row r="106" spans="1:5" s="6" customFormat="1">
+      <c r="A106" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="B105" s="8"/>
-      <c r="C105" s="8"/>
-      <c r="D105" s="8"/>
-      <c r="E105" s="8"/>
-    </row>
-    <row r="106" spans="1:5" s="6" customFormat="1" ht="31.5">
-      <c r="B106" s="6" t="s">
+      <c r="B106" s="8"/>
+      <c r="C106" s="8"/>
+      <c r="D106" s="8"/>
+      <c r="E106" s="8"/>
+    </row>
+    <row r="107" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B107" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="E106" s="3" t="s">
+      <c r="E107" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="107" spans="1:5" s="6" customFormat="1" ht="31.5">
-      <c r="B107" s="4" t="s">
+    <row r="108" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B108" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="E107" s="3" t="s">
+      <c r="E108" s="3" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="31.5">
-      <c r="A108" s="2" t="s">
+    <row r="109" spans="1:5" ht="30">
+      <c r="A109" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B108" s="18"/>
-      <c r="C108" s="18"/>
-      <c r="D108" s="14"/>
-      <c r="E108" s="19"/>
-    </row>
-    <row r="109" spans="1:5" s="15" customFormat="1" ht="47.25">
-      <c r="B109" s="15" t="s">
+      <c r="B109" s="18"/>
+      <c r="C109" s="18"/>
+      <c r="D109" s="14"/>
+      <c r="E109" s="19"/>
+    </row>
+    <row r="110" spans="1:5" s="15" customFormat="1" ht="30">
+      <c r="B110" s="15" t="s">
         <v>145</v>
-      </c>
-      <c r="D109" s="16"/>
-      <c r="E109" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" s="15" customFormat="1" ht="47.25">
-      <c r="B110" s="15" t="s">
-        <v>146</v>
       </c>
       <c r="D110" s="16"/>
       <c r="E110" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" s="15" customFormat="1" ht="47.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="B111" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D111" s="16"/>
       <c r="E111" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" s="15" customFormat="1" ht="47.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="B112" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D112" s="16"/>
       <c r="E112" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="113" spans="2:5" s="15" customFormat="1" ht="47.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" s="15" customFormat="1" ht="45">
       <c r="B113" s="15" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D113" s="16"/>
       <c r="E113" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="114" spans="2:5" s="15" customFormat="1" ht="47.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" s="15" customFormat="1" ht="45">
       <c r="B114" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D114" s="16"/>
       <c r="E114" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5" s="15" customFormat="1" ht="45">
+      <c r="B115" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D115" s="16"/>
+      <c r="E115" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="115" spans="2:5" s="6" customFormat="1">
-      <c r="E115" s="9"/>
-    </row>
-    <row r="116" spans="2:5" s="6" customFormat="1"/>
+    <row r="116" spans="2:5" s="6" customFormat="1">
+      <c r="E116" s="9"/>
+    </row>
     <row r="117" spans="2:5" s="6" customFormat="1"/>
     <row r="118" spans="2:5" s="6" customFormat="1"/>
     <row r="119" spans="2:5" s="6" customFormat="1"/>
@@ -4443,6 +4478,7 @@
     <row r="122" spans="2:5" s="6" customFormat="1"/>
     <row r="123" spans="2:5" s="6" customFormat="1"/>
     <row r="124" spans="2:5" s="6" customFormat="1"/>
+    <row r="125" spans="2:5" s="6" customFormat="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Fixed "RaceCode" to be a Pima County Code.  Added Pima County Sample XML Instances for Custody Status Change and Custody Release.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReport.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="4380" yWindow="280" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Booking Report" sheetId="1" r:id="rId1"/>
@@ -813,10 +813,10 @@
     <t>/br-doc:BookingReport/j:Offense[@structures:id=/br-doc:BookingReport/j:OffenseChargeAssociation/j:Offense/@structures:ref]/j:OffenseCategoryText</t>
   </si>
   <si>
-    <t>Race Code (Adams County)</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/ac-bkg-codes:PersonRaceCode</t>
+    <t>Race Code (Pima County)</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/pc-bkg-codes:PersonRaceCode</t>
   </si>
 </sst>
 </file>
@@ -3181,8 +3181,8 @@
   <dimension ref="A1:E125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Added "ChargeSeverityText" and "ChargeJurisdictionCourt" to the Booking and Custody Status Change SSPs.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReport.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="280" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="6700" yWindow="2580" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Booking Report" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="268">
   <si>
     <t>Race</t>
   </si>
@@ -312,12 +312,6 @@
     <t>Arrest Location Long</t>
   </si>
   <si>
-    <t>Case</t>
-  </si>
-  <si>
-    <t>Case Court Name</t>
-  </si>
-  <si>
     <t>/br-doc:BookingReport/nc:DocumentCreationDate/nc:DateTime</t>
   </si>
   <si>
@@ -696,9 +690,6 @@
     <t>/br-doc:BookingReport/br-ext:CareEpisode[@structures:id=/br-doc:BookingReport/nc:Person/br-ext:PersonCareEpisode/@structures:ref]/nc:ActivityDateRange/nc:EndDate/nc:Date</t>
   </si>
   <si>
-    <t>/br-doc:BookingReport/nc:Case[@structures:id=/br-doc:BookingReport/j:ActivityCaseAssociation/nc:Case/@structures:ref]/j:CaseAugmentation/j:CaseCourt/j:CourtName</t>
-  </si>
-  <si>
     <t>/br-doc:BookingReport/j:Booking[@structures:id=/br-doc:BookingReport/j:ActivityCaseAssociation/nc:Activity/@structures:ref]/j:BookingSubject/j:SubjectIdentification/nc:IdentificationID</t>
   </si>
   <si>
@@ -817,6 +808,21 @@
   </si>
   <si>
     <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/pc-bkg-codes:PersonRaceCode</t>
+  </si>
+  <si>
+    <t>Charge Severity</t>
+  </si>
+  <si>
+    <t>Severity Text</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Charge[@structures:id=/br-doc:BookingReport/j:Arrest/j:ArrestCharge/@structures:ref]/j:ChargeSeverityText</t>
+  </si>
+  <si>
+    <t>Charge Jurisdiction Court</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Charge[@structures:id=/br-doc:BookingReport/j:Arrest/j:ArrestCharge/@structures:ref]/br-ext:ChargeJurisdictionCourt/j:CourtName</t>
   </si>
 </sst>
 </file>
@@ -935,9 +941,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="916">
+  <cellStyleXfs count="924">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1928,7 +1942,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="916">
+  <cellStyles count="924">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2386,6 +2400,10 @@
     <cellStyle name="Followed Hyperlink" xfId="911" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="913" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="915" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="917" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="919" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="921" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="923" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2843,6 +2861,10 @@
     <cellStyle name="Hyperlink" xfId="910" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="912" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="914" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="916" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="918" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="920" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="922" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3181,8 +3203,8 @@
   <dimension ref="A1:E125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <pane ySplit="2" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3239,7 +3261,7 @@
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="6" customFormat="1">
@@ -3252,7 +3274,7 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="6" customFormat="1">
@@ -3274,7 +3296,7 @@
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="6" customFormat="1">
@@ -3287,12 +3309,12 @@
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="6" customFormat="1">
       <c r="A9" s="7" t="s">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -3302,38 +3324,40 @@
     <row r="10" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="6" customFormat="1">
-      <c r="A11" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="1:5" s="6" customFormat="1" ht="45">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="6" customFormat="1" ht="45">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -3341,7 +3365,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="6" customFormat="1" ht="30">
+    <row r="14" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
         <v>138</v>
@@ -3352,7 +3376,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="6" customFormat="1" ht="30">
+    <row r="15" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
         <v>139</v>
@@ -3368,96 +3392,100 @@
       <c r="B16" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>141</v>
+      </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="6" customFormat="1" ht="45">
+    <row r="17" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C17" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="6" customFormat="1" ht="45">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>142</v>
+        <v>2</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>143</v>
+        <v>28</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>159</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3" t="s">
-        <v>2</v>
+    <row r="20" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A20" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>261</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="3"/>
+        <v>29</v>
+      </c>
       <c r="E20" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="6" customFormat="1" ht="30">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="D21" s="3"/>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="10" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A22" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="10" t="s">
@@ -3467,10 +3495,10 @@
     <row r="24" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="10" t="s">
@@ -3480,461 +3508,459 @@
     <row r="25" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="10" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="6" customFormat="1" ht="45">
+    <row r="26" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>51</v>
+        <v>127</v>
       </c>
       <c r="D26" s="3"/>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="10" t="s">
+    <row r="27" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" s="11"/>
+      <c r="E27" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3" t="s">
+    <row r="28" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A29" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="4" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A30" s="4"/>
       <c r="B30" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C30" s="4"/>
+        <v>77</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A31" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="A31" s="4"/>
       <c r="B31" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A32" s="4"/>
       <c r="B32" s="4" t="s">
-        <v>77</v>
+        <v>178</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>83</v>
+        <v>179</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
-        <v>115</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="6" customFormat="1">
-      <c r="A36" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
+    <row r="34" spans="1:5" s="6" customFormat="1">
+      <c r="A34" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+    </row>
+    <row r="35" spans="1:5" s="6" customFormat="1" ht="60">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="6" customFormat="1" ht="60">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="22" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="37" spans="1:5" s="6" customFormat="1" ht="60">
       <c r="A37" s="3"/>
       <c r="B37" s="3" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="22" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="6" customFormat="1" ht="60">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="22" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="6" customFormat="1" ht="60">
       <c r="A39" s="3"/>
       <c r="B39" s="3" t="s">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>51</v>
+        <v>127</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="22" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" s="6" customFormat="1" ht="60">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D40" s="3"/>
-      <c r="E40" s="22" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="6" customFormat="1" ht="60">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D41" s="3"/>
-      <c r="E41" s="22" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" s="6" customFormat="1">
-      <c r="A42" s="7" t="s">
+    <row r="40" spans="1:5" s="6" customFormat="1">
+      <c r="A40" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-    </row>
-    <row r="43" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B43" s="4" t="s">
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+    </row>
+    <row r="41" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B41" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C41" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="E41" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B42" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="6" customFormat="1" ht="75">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D43" s="5"/>
       <c r="E43" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B44" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="E44" s="3" t="s">
+    <row r="44" spans="1:5" s="6" customFormat="1">
+      <c r="A44" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+    </row>
+    <row r="45" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A45" s="23"/>
+      <c r="B45" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="6" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" s="9" customFormat="1" ht="45">
+      <c r="B46" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" s="6" customFormat="1">
+      <c r="A49" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+    </row>
+    <row r="50" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B50" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="6" customFormat="1" ht="75">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D45" s="5"/>
-      <c r="E45" s="3" t="s">
+    <row r="51" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B51" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="6" customFormat="1">
-      <c r="A46" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
-    </row>
-    <row r="47" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A47" s="23"/>
-      <c r="B47" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="6" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" s="9" customFormat="1" ht="45">
-      <c r="B48" s="21" t="s">
-        <v>252</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E48" s="6" t="s">
+    <row r="52" spans="1:5" s="6" customFormat="1">
+      <c r="A52" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+    </row>
+    <row r="53" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B53" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B54" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E54" s="3" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3" t="s">
+    <row r="55" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B55" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E55" s="3" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3" t="s">
+    <row r="56" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A56" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E56" s="9" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="6" customFormat="1">
-      <c r="A51" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-    </row>
-    <row r="52" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B52" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B53" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" s="6" customFormat="1">
-      <c r="A54" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B54" s="8"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
-    </row>
-    <row r="55" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B55" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="C55" s="6" t="s">
+    <row r="57" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B57" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C57" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E55" s="3" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B56" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="E56" s="3" t="s">
+      <c r="E57" s="6" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B57" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E57" s="3" t="s">
+    <row r="58" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B58" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E58" s="3" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A58" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E58" s="9" t="s">
+    <row r="59" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B59" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E59" s="3" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B59" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E59" s="6" t="s">
+    <row r="60" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B60" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E60" s="3" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B60" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E60" s="3" t="s">
+    <row r="61" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A61" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E61" s="9" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="61" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B61" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E61" s="3" t="s">
+    <row r="62" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A62" s="5"/>
+      <c r="B62" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D62" s="5"/>
+      <c r="E62" s="9" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="62" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B62" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E62" s="3" t="s">
+    <row r="63" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="A63" s="5"/>
+      <c r="B63" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="9" t="s">
         <v>235</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A63" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E63" s="9" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="64" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3942,167 +3968,164 @@
       <c r="B64" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="C64" s="5" t="s">
-        <v>177</v>
-      </c>
+      <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="A65" s="5"/>
+      <c r="A65" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="B65" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C65" s="5"/>
+        <v>73</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="D65" s="5"/>
       <c r="E65" s="9" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A66" s="5"/>
+        <v>237</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="A66" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="B66" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="C66" s="5"/>
+        <v>74</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>86</v>
+      </c>
       <c r="D66" s="5"/>
       <c r="E66" s="9" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="A67" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D67" s="5"/>
-      <c r="E67" s="9" t="s">
-        <v>240</v>
-      </c>
+        <v>238</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="6" customFormat="1">
+      <c r="A67" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="B67" s="8"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="8"/>
     </row>
     <row r="68" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="A68" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D68" s="5"/>
-      <c r="E68" s="9" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" s="6" customFormat="1">
-      <c r="A69" s="7" t="s">
+      <c r="B68" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="B69" s="8"/>
-      <c r="C69" s="8"/>
-      <c r="D69" s="8"/>
-      <c r="E69" s="8"/>
+      <c r="C68" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B69" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="70" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="B70" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="C70" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="C70" s="6" t="s">
-        <v>258</v>
-      </c>
       <c r="E70" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B71" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>262</v>
-      </c>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" s="6" customFormat="1">
+      <c r="A71" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B71" s="8"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="8"/>
     </row>
     <row r="72" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="B72" s="4" t="s">
-        <v>256</v>
+        <v>13</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>260</v>
+        <v>40</v>
       </c>
       <c r="E72" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B73" s="4" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" s="6" customFormat="1">
-      <c r="A73" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B73" s="8"/>
-      <c r="C73" s="8"/>
-      <c r="D73" s="8"/>
-      <c r="E73" s="8"/>
+      <c r="C73" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="74" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="B74" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E74" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B75" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" s="6" customFormat="1" ht="105">
+      <c r="A76" s="5"/>
+      <c r="B76" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B75" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B76" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" s="6" customFormat="1" ht="105">
-      <c r="A77" s="5"/>
+    <row r="77" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="A77" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="B77" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>71</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="C77" s="5"/>
       <c r="D77" s="5"/>
-      <c r="E77" s="5" t="s">
-        <v>246</v>
+      <c r="E77" s="9" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="78" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="A78" s="6" t="s">
-        <v>37</v>
-      </c>
       <c r="B78" s="6" t="s">
         <v>66</v>
       </c>
@@ -4110,7 +4133,7 @@
         <v>65</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="79" spans="1:5" s="6" customFormat="1" ht="30">
@@ -4118,13 +4141,13 @@
         <v>37</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="80" spans="1:5" s="6" customFormat="1">
@@ -4139,56 +4162,56 @@
     <row r="81" spans="1:5" s="12" customFormat="1" ht="45">
       <c r="A81" s="5"/>
       <c r="B81" s="20" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
       <c r="E81" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="82" spans="1:5" s="12" customFormat="1" ht="30">
       <c r="A82" s="5"/>
       <c r="B82" s="20" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
       <c r="E82" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="83" spans="1:5" s="12" customFormat="1" ht="30">
       <c r="A83" s="5"/>
       <c r="B83" s="20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
       <c r="E83" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="84" spans="1:5" s="12" customFormat="1" ht="45">
       <c r="A84" s="5"/>
       <c r="B84" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
       <c r="E84" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="85" spans="1:5" s="12" customFormat="1" ht="30">
       <c r="A85" s="5"/>
       <c r="B85" s="20" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
       <c r="E85" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="86" spans="1:5" s="6" customFormat="1" ht="45">
@@ -4199,7 +4222,7 @@
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
       <c r="E86" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="87" spans="1:5" s="6" customFormat="1" ht="45">
@@ -4210,7 +4233,7 @@
       <c r="C87" s="5"/>
       <c r="D87" s="5"/>
       <c r="E87" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="88" spans="1:5" s="6" customFormat="1" ht="30">
@@ -4221,12 +4244,12 @@
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
       <c r="E88" s="4" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="89" spans="1:5" s="6" customFormat="1">
       <c r="A89" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B89" s="8"/>
       <c r="C89" s="8"/>
@@ -4235,153 +4258,153 @@
     </row>
     <row r="90" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B90" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="91" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B91" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C91" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="C91" s="6" t="s">
-        <v>185</v>
-      </c>
       <c r="E91" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B92" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="93" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B93" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="94" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B94" s="6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="95" spans="1:5" s="6" customFormat="1" ht="60">
       <c r="B95" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="96" spans="1:5" s="6" customFormat="1" ht="60">
       <c r="B96" s="6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="97" spans="1:5" s="6" customFormat="1" ht="60">
       <c r="B97" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="98" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B98" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="99" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B99" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="100" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B100" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="101" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B101" s="6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="102" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B102" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="103" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B103" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="104" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B104" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="105" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B105" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="106" spans="1:5" s="6" customFormat="1">
       <c r="A106" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B106" s="8"/>
       <c r="C106" s="8"/>
@@ -4390,23 +4413,23 @@
     </row>
     <row r="107" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="B107" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="108" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="B108" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="30">
       <c r="A109" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B109" s="18"/>
       <c r="C109" s="18"/>
@@ -4415,56 +4438,56 @@
     </row>
     <row r="110" spans="1:5" s="15" customFormat="1" ht="30">
       <c r="B110" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D110" s="16"/>
       <c r="E110" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="111" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="B111" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D111" s="16"/>
       <c r="E111" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="112" spans="1:5" s="15" customFormat="1" ht="45">
       <c r="B112" s="15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D112" s="16"/>
       <c r="E112" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="113" spans="2:5" s="15" customFormat="1" ht="45">
       <c r="B113" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D113" s="16"/>
       <c r="E113" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="114" spans="2:5" s="15" customFormat="1" ht="45">
       <c r="B114" s="15" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D114" s="16"/>
       <c r="E114" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="115" spans="2:5" s="15" customFormat="1" ht="45">
       <c r="B115" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D115" s="16"/>
       <c r="E115" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="116" spans="2:5" s="6" customFormat="1">

</xml_diff>

<commit_message>
Added Pima County Person Ethnicity Codes and Charge Disposition (/nc:DispositionText)to Booking and Custody Status Change SSPs.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReport.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6700" yWindow="2580" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="3940" yWindow="520" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Booking Report" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="273">
   <si>
     <t>Race</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Person DOB</t>
   </si>
   <si>
-    <t>Person Ethnicity</t>
-  </si>
-  <si>
     <t>Person Race</t>
   </si>
   <si>
@@ -823,6 +820,24 @@
   </si>
   <si>
     <t>/br-doc:BookingReport/j:Charge[@structures:id=/br-doc:BookingReport/j:Arrest/j:ArrestCharge/@structures:ref]/br-ext:ChargeJurisdictionCourt/j:CourtName</t>
+  </si>
+  <si>
+    <t>Person Ethnicity Code</t>
+  </si>
+  <si>
+    <t>Person Ethnicity Code (Pima County)</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/pc-bkg-codes:PersonEthnicityCode</t>
+  </si>
+  <si>
+    <t>Charge Disposition</t>
+  </si>
+  <si>
+    <t>ChargeDisposition Text</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Charge[@structures:id=/br-doc:BookingReport/j:Arrest/j:ArrestCharge/@structures:ref]/j:ChargeDisposition/nc:DispositionText</t>
   </si>
 </sst>
 </file>
@@ -941,9 +956,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="924">
+  <cellStyleXfs count="934">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1942,7 +1967,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="924">
+  <cellStyles count="934">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2404,6 +2429,11 @@
     <cellStyle name="Followed Hyperlink" xfId="919" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="921" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="923" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="925" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="927" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="929" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="931" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="933" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2865,6 +2895,11 @@
     <cellStyle name="Hyperlink" xfId="918" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="920" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="922" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="924" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="926" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="928" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="930" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="932" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3200,11 +3235,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E125"/>
+  <dimension ref="A1:E127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E77" sqref="E77"/>
+      <pane ySplit="2" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3218,7 +3253,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="36" customHeight="1">
       <c r="A1" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="13"/>
@@ -3236,7 +3271,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>10</v>
@@ -3261,7 +3296,7 @@
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="6" customFormat="1">
@@ -3274,12 +3309,12 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="6" customFormat="1">
       <c r="A6" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -3296,7 +3331,7 @@
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="6" customFormat="1">
@@ -3309,12 +3344,12 @@
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="6" customFormat="1">
       <c r="A9" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -3324,80 +3359,80 @@
     <row r="10" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="6" customFormat="1" ht="30">
@@ -3410,177 +3445,179 @@
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="6" customFormat="1" ht="30">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="6" customFormat="1" ht="52" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>28</v>
+        <v>267</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="A19" s="3"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A19" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="B19" s="3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>29</v>
+        <v>268</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A20" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="6" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A21" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>261</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="10" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="6" customFormat="1" ht="30">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="C27" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A28" s="4"/>
       <c r="B28" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
+        <v>86</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="11"/>
       <c r="E28" s="4" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A29" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="A29" s="4"/>
       <c r="B29" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>81</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A30" s="4"/>
+      <c r="A30" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="B30" s="4" t="s">
         <v>77</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="6" customFormat="1" ht="45">
@@ -3599,902 +3636,924 @@
     <row r="32" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A32" s="4"/>
       <c r="B32" s="4" t="s">
-        <v>178</v>
+        <v>75</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>179</v>
+        <v>81</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
-        <v>180</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
-        <v>75</v>
+        <v>177</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>84</v>
+        <v>178</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="6" customFormat="1">
-      <c r="A34" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-    </row>
-    <row r="35" spans="1:5" s="6" customFormat="1" ht="60">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="22" t="s">
-        <v>132</v>
-      </c>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="6" customFormat="1">
+      <c r="A35" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
     </row>
     <row r="36" spans="1:5" s="6" customFormat="1" ht="60">
       <c r="A36" s="3"/>
       <c r="B36" s="3" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="22" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="6" customFormat="1" ht="60">
       <c r="A37" s="3"/>
       <c r="B37" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="22" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="6" customFormat="1" ht="60">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="22" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="6" customFormat="1" ht="60">
       <c r="A39" s="3"/>
       <c r="B39" s="3" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>127</v>
+        <v>51</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="22" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" s="6" customFormat="1">
-      <c r="A40" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="6" customFormat="1" ht="60">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="6" customFormat="1">
+      <c r="A41" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-    </row>
-    <row r="41" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B41" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>116</v>
-      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="B42" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B43" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="E42" s="3" t="s">
+      <c r="C43" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="6" customFormat="1" ht="75">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D44" s="5"/>
+      <c r="E44" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="6" customFormat="1" ht="75">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D43" s="5"/>
-      <c r="E43" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" s="6" customFormat="1">
-      <c r="A44" s="7" t="s">
+    <row r="45" spans="1:5" s="6" customFormat="1">
+      <c r="A45" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-    </row>
-    <row r="45" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A45" s="23"/>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+    </row>
+    <row r="46" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A46" s="23"/>
+      <c r="B46" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="6" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" s="9" customFormat="1" ht="45">
+      <c r="B47" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="6" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" s="9" customFormat="1" ht="45">
-      <c r="B46" s="21" t="s">
-        <v>249</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="C47" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A48" s="3"/>
       <c r="B48" s="3" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" s="6" customFormat="1">
-      <c r="A49" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-    </row>
-    <row r="50" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B50" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="E50" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" s="6" customFormat="1">
+      <c r="A50" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+    </row>
+    <row r="51" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B51" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B52" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B51" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" s="6" customFormat="1">
-      <c r="A52" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8"/>
-    </row>
-    <row r="53" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B53" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>247</v>
-      </c>
+    <row r="53" spans="1:5" s="6" customFormat="1">
+      <c r="A53" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
     </row>
     <row r="54" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B54" s="4" t="s">
-        <v>92</v>
+        <v>245</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>148</v>
+        <v>33</v>
       </c>
       <c r="E54" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B55" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B56" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E56" s="3" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B55" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E55" s="3" t="s">
+    <row r="57" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A57" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E57" s="9" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A56" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E56" s="9" t="s">
+    <row r="58" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B58" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E58" s="6" t="s">
         <v>228</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B57" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B58" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B59" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B60" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B61" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C61" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="E61" s="3" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B60" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C60" s="6" t="s">
+    <row r="62" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A62" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B62" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="C62" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E62" s="9" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="61" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A61" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A62" s="5"/>
-      <c r="B62" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="D62" s="5"/>
-      <c r="E62" s="9" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" s="6" customFormat="1" ht="30">
+    <row r="63" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A63" s="5"/>
       <c r="B63" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C63" s="5"/>
+        <v>173</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>174</v>
+      </c>
       <c r="D63" s="5"/>
       <c r="E63" s="9" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" s="6" customFormat="1" ht="45">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A64" s="5"/>
       <c r="B64" s="5" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="9" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="A65" s="5" t="s">
-        <v>37</v>
-      </c>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A65" s="5"/>
       <c r="B65" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>85</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="9" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A66" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="9" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" s="6" customFormat="1">
-      <c r="A67" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="B67" s="8"/>
-      <c r="C67" s="8"/>
-      <c r="D67" s="8"/>
-      <c r="E67" s="8"/>
-    </row>
-    <row r="68" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B68" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="C68" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>258</v>
-      </c>
+        <v>236</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="A67" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D67" s="5"/>
+      <c r="E67" s="9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="6" customFormat="1">
+      <c r="A68" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="B68" s="8"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
     </row>
     <row r="69" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="B69" s="4" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="70" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="B70" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" s="6" customFormat="1">
-      <c r="A71" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B71" s="8"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="8"/>
-      <c r="E71" s="8"/>
-    </row>
-    <row r="72" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B72" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>240</v>
-      </c>
+        <v>258</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B71" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="6" customFormat="1">
+      <c r="A72" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B72" s="8"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
     </row>
     <row r="73" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="B73" s="4" t="s">
-        <v>263</v>
+        <v>13</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>264</v>
+        <v>39</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>265</v>
+        <v>239</v>
       </c>
     </row>
     <row r="74" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="B74" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B75" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C74" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E74" s="3" t="s">
+      <c r="C75" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B76" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B77" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E77" s="3" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B75" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E75" s="3" t="s">
+    <row r="78" spans="1:5" s="6" customFormat="1" ht="105">
+      <c r="A78" s="5"/>
+      <c r="B78" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5" t="s">
         <v>242</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" s="6" customFormat="1" ht="105">
-      <c r="A76" s="5"/>
-      <c r="B76" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="A77" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="9" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B78" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="79" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A79" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>135</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
       <c r="E79" s="9" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" s="6" customFormat="1">
-      <c r="A80" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B80" s="8"/>
-      <c r="C80" s="8"/>
-      <c r="D80" s="8"/>
-      <c r="E80" s="8"/>
-    </row>
-    <row r="81" spans="1:5" s="12" customFormat="1" ht="45">
-      <c r="A81" s="5"/>
-      <c r="B81" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="C81" s="5"/>
-      <c r="D81" s="5"/>
-      <c r="E81" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" s="12" customFormat="1" ht="30">
-      <c r="A82" s="5"/>
-      <c r="B82" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="C82" s="5"/>
-      <c r="D82" s="5"/>
-      <c r="E82" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" s="12" customFormat="1" ht="30">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B80" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="A81" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" s="6" customFormat="1">
+      <c r="A82" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B82" s="8"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="8"/>
+    </row>
+    <row r="83" spans="1:5" s="12" customFormat="1" ht="45">
       <c r="A83" s="5"/>
       <c r="B83" s="20" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
       <c r="E83" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" s="12" customFormat="1" ht="45">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" s="12" customFormat="1" ht="30">
       <c r="A84" s="5"/>
       <c r="B84" s="20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
       <c r="E84" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="85" spans="1:5" s="12" customFormat="1" ht="30">
       <c r="A85" s="5"/>
       <c r="B85" s="20" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
       <c r="E85" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" s="6" customFormat="1" ht="45">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" s="12" customFormat="1" ht="45">
       <c r="A86" s="5"/>
       <c r="B86" s="20" t="s">
-        <v>95</v>
+        <v>166</v>
       </c>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
       <c r="E86" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" s="6" customFormat="1" ht="45">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" s="12" customFormat="1" ht="30">
       <c r="A87" s="5"/>
       <c r="B87" s="20" t="s">
-        <v>96</v>
+        <v>167</v>
       </c>
       <c r="C87" s="5"/>
       <c r="D87" s="5"/>
       <c r="E87" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" s="6" customFormat="1" ht="30">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A88" s="5"/>
-      <c r="B88" s="5" t="s">
-        <v>69</v>
+      <c r="B88" s="20" t="s">
+        <v>94</v>
       </c>
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
       <c r="E88" s="4" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" s="6" customFormat="1">
-      <c r="A89" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B89" s="8"/>
-      <c r="C89" s="8"/>
-      <c r="D89" s="8"/>
-      <c r="E89" s="8"/>
-    </row>
-    <row r="90" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B90" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B91" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="E91" s="3" t="s">
-        <v>206</v>
-      </c>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A89" s="5"/>
+      <c r="B89" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C89" s="5"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="A90" s="5"/>
+      <c r="B90" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C90" s="5"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" s="6" customFormat="1">
+      <c r="A91" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B91" s="8"/>
+      <c r="C91" s="8"/>
+      <c r="D91" s="8"/>
+      <c r="E91" s="8"/>
     </row>
     <row r="92" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B92" s="6" t="s">
-        <v>184</v>
+        <v>125</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="93" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B93" s="6" t="s">
-        <v>186</v>
+      <c r="B93" s="4" t="s">
+        <v>180</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="94" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B94" s="6" t="s">
-        <v>188</v>
+        <v>183</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>184</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" s="6" customFormat="1" ht="60">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B95" s="6" t="s">
-        <v>189</v>
+        <v>185</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>186</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" s="6" customFormat="1" ht="60">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B96" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="97" spans="1:5" s="6" customFormat="1" ht="60">
       <c r="B97" s="6" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" s="6" customFormat="1" ht="45">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" s="6" customFormat="1" ht="60">
       <c r="B98" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="C98" s="6" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" s="6" customFormat="1" ht="45">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" s="6" customFormat="1" ht="60">
       <c r="B99" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="C99" s="6" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="100" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B100" s="6" t="s">
-        <v>196</v>
+        <v>191</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>192</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="101" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B101" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>194</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="102" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B102" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="103" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B103" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B104" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B105" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B106" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="E103" s="3" t="s">
+      <c r="E106" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B107" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="E107" s="3" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="104" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B104" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="E104" s="3" t="s">
+    <row r="108" spans="1:5" s="6" customFormat="1">
+      <c r="A108" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B108" s="8"/>
+      <c r="C108" s="8"/>
+      <c r="D108" s="8"/>
+      <c r="E108" s="8"/>
+    </row>
+    <row r="109" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B109" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="E109" s="3" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="105" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B105" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="E105" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" s="6" customFormat="1">
-      <c r="A106" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="B106" s="8"/>
-      <c r="C106" s="8"/>
-      <c r="D106" s="8"/>
-      <c r="E106" s="8"/>
-    </row>
-    <row r="107" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B107" s="6" t="s">
+    <row r="110" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B110" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="E107" s="3" t="s">
+      <c r="E110" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="108" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B108" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="E108" s="3" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" ht="30">
-      <c r="A109" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B109" s="18"/>
-      <c r="C109" s="18"/>
-      <c r="D109" s="14"/>
-      <c r="E109" s="19"/>
-    </row>
-    <row r="110" spans="1:5" s="15" customFormat="1" ht="30">
-      <c r="B110" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="D110" s="16"/>
-      <c r="E110" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" s="15" customFormat="1" ht="45">
-      <c r="B111" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="D111" s="16"/>
-      <c r="E111" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" s="15" customFormat="1" ht="45">
+    <row r="111" spans="1:5" ht="30">
+      <c r="A111" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B111" s="18"/>
+      <c r="C111" s="18"/>
+      <c r="D111" s="14"/>
+      <c r="E111" s="19"/>
+    </row>
+    <row r="112" spans="1:5" s="15" customFormat="1" ht="30">
       <c r="B112" s="15" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D112" s="16"/>
       <c r="E112" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="113" spans="2:5" s="15" customFormat="1" ht="45">
       <c r="B113" s="15" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D113" s="16"/>
       <c r="E113" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="114" spans="2:5" s="15" customFormat="1" ht="45">
       <c r="B114" s="15" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D114" s="16"/>
       <c r="E114" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="115" spans="2:5" s="15" customFormat="1" ht="45">
       <c r="B115" s="15" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D115" s="16"/>
       <c r="E115" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="116" spans="2:5" s="6" customFormat="1">
-      <c r="E116" s="9"/>
-    </row>
-    <row r="117" spans="2:5" s="6" customFormat="1"/>
-    <row r="118" spans="2:5" s="6" customFormat="1"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5" s="15" customFormat="1" ht="45">
+      <c r="B116" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="D116" s="16"/>
+      <c r="E116" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="117" spans="2:5" s="15" customFormat="1" ht="45">
+      <c r="B117" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="D117" s="16"/>
+      <c r="E117" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5" s="6" customFormat="1">
+      <c r="E118" s="9"/>
+    </row>
     <row r="119" spans="2:5" s="6" customFormat="1"/>
     <row r="120" spans="2:5" s="6" customFormat="1"/>
     <row r="121" spans="2:5" s="6" customFormat="1"/>
@@ -4502,6 +4561,8 @@
     <row r="123" spans="2:5" s="6" customFormat="1"/>
     <row r="124" spans="2:5" s="6" customFormat="1"/>
     <row r="125" spans="2:5" s="6" customFormat="1"/>
+    <row r="126" spans="2:5" s="6" customFormat="1"/>
+    <row r="127" spans="2:5" s="6" customFormat="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Added "SubjectLocationStatus/nc:StatusDescriptionText" to Booking and CustodyStatusChange Reporting SSPs.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReport.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3940" yWindow="520" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="4220" yWindow="2520" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Booking Report" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="276">
   <si>
     <t>Race</t>
   </si>
@@ -838,6 +838,15 @@
   </si>
   <si>
     <t>/br-doc:BookingReport/j:Charge[@structures:id=/br-doc:BookingReport/j:Arrest/j:ArrestCharge/@structures:ref]/j:ChargeDisposition/nc:DispositionText</t>
+  </si>
+  <si>
+    <t>Booking Subject Location Status Description</t>
+  </si>
+  <si>
+    <t>Current location status of the booking subject at the time of report</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Booking[@structures:id=/br-doc:BookingReport/j:ActivityCaseAssociation/nc:Activity/@structures:ref]/j:BookingSubject/br-ext:SubjectLocationStatus/nc:StatusDescriptionText</t>
   </si>
 </sst>
 </file>
@@ -956,9 +965,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="934">
+  <cellStyleXfs count="936">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1967,7 +1978,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="934">
+  <cellStyles count="936">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2434,6 +2445,7 @@
     <cellStyle name="Followed Hyperlink" xfId="929" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="931" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="933" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="935" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2900,6 +2912,7 @@
     <cellStyle name="Hyperlink" xfId="928" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="930" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="932" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="934" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3235,17 +3248,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E127"/>
+  <dimension ref="A1:E128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D71" sqref="D71"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.33203125" style="17" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" style="17" customWidth="1"/>
     <col min="3" max="4" width="28.33203125" style="17" customWidth="1"/>
     <col min="5" max="5" width="92.33203125" style="17" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="17"/>
@@ -3821,222 +3834,218 @@
         <v>222</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" s="6" customFormat="1" ht="45">
+    <row r="48" spans="1:5" s="9" customFormat="1" ht="45">
+      <c r="B48" s="21" t="s">
+        <v>273</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A49" s="3"/>
       <c r="B49" s="3" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="6" customFormat="1">
-      <c r="A50" s="7" t="s">
+    <row r="51" spans="1:5" s="6" customFormat="1">
+      <c r="A51" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-    </row>
-    <row r="51" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+    </row>
+    <row r="52" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B52" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="E52" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B52" s="4" t="s">
+    <row r="53" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B53" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C52" s="6" t="s">
+      <c r="C53" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E53" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="6" customFormat="1">
-      <c r="A53" s="7" t="s">
+    <row r="54" spans="1:5" s="6" customFormat="1">
+      <c r="A54" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="8"/>
-    </row>
-    <row r="54" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B54" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>246</v>
-      </c>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
     </row>
     <row r="55" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B55" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B56" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C56" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E56" s="3" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B56" s="4" t="s">
+    <row r="57" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B57" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="C57" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E57" s="3" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A57" s="6" t="s">
+    <row r="58" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A58" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B58" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C58" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E57" s="9" t="s">
+      <c r="E58" s="9" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B58" s="4" t="s">
+    <row r="59" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B59" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C59" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E58" s="6" t="s">
+      <c r="E59" s="6" t="s">
         <v>228</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B59" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="60" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B60" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B61" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C61" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="E61" s="3" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="61" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B61" s="6" t="s">
+    <row r="62" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B62" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C62" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E62" s="3" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="62" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A62" s="6" t="s">
+    <row r="63" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A63" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="B63" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C63" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E62" s="9" t="s">
+      <c r="E63" s="9" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="D63" s="5"/>
-      <c r="E63" s="9" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" s="6" customFormat="1" ht="30">
+    <row r="64" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A64" s="5"/>
       <c r="B64" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C64" s="5"/>
+        <v>173</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>174</v>
+      </c>
       <c r="D64" s="5"/>
       <c r="E64" s="9" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" s="6" customFormat="1" ht="45">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A65" s="5"/>
       <c r="B65" s="5" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="9" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="A66" s="5" t="s">
-        <v>36</v>
-      </c>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="A66" s="5"/>
       <c r="B66" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>84</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="67" spans="1:5" s="6" customFormat="1" ht="30">
@@ -4044,517 +4053,531 @@
         <v>36</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="9" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="A68" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D68" s="5"/>
+      <c r="E68" s="9" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="68" spans="1:5" s="6" customFormat="1">
-      <c r="A68" s="7" t="s">
+    <row r="69" spans="1:5" s="6" customFormat="1">
+      <c r="A69" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="B68" s="8"/>
-      <c r="C68" s="8"/>
-      <c r="D68" s="8"/>
-      <c r="E68" s="8"/>
-    </row>
-    <row r="69" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B69" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>257</v>
-      </c>
+      <c r="B69" s="8"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="8"/>
     </row>
     <row r="70" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="B70" s="4" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="71" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="B71" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B72" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="C71" s="6" t="s">
+      <c r="C72" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="E71" s="3" t="s">
+      <c r="E72" s="3" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="72" spans="1:5" s="6" customFormat="1">
-      <c r="A72" s="7" t="s">
+    <row r="73" spans="1:5" s="6" customFormat="1">
+      <c r="A73" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B72" s="8"/>
-      <c r="C72" s="8"/>
-      <c r="D72" s="8"/>
-      <c r="E72" s="8"/>
-    </row>
-    <row r="73" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B73" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>239</v>
-      </c>
+      <c r="B73" s="8"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="8"/>
+      <c r="E73" s="8"/>
     </row>
     <row r="74" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="B74" s="4" t="s">
-        <v>262</v>
+        <v>13</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>263</v>
+        <v>39</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>264</v>
+        <v>239</v>
       </c>
     </row>
     <row r="75" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="B75" s="4" t="s">
-        <v>9</v>
+        <v>262</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>30</v>
+        <v>263</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>240</v>
+        <v>264</v>
       </c>
     </row>
     <row r="76" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="B76" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B77" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="C76" s="6" t="s">
+      <c r="C77" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="E76" s="3" t="s">
+      <c r="E77" s="3" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="77" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B77" s="4" t="s">
+    <row r="78" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B78" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C77" s="6" t="s">
+      <c r="C78" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E77" s="3" t="s">
+      <c r="E78" s="3" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="78" spans="1:5" s="6" customFormat="1" ht="105">
-      <c r="A78" s="5"/>
-      <c r="B78" s="5" t="s">
+    <row r="79" spans="1:5" s="6" customFormat="1" ht="105">
+      <c r="A79" s="5"/>
+      <c r="B79" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C78" s="5" t="s">
+      <c r="C79" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5" t="s">
+      <c r="D79" s="5"/>
+      <c r="E79" s="5" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="79" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="A79" s="6" t="s">
+    <row r="80" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="A80" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B80" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="9" t="s">
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="9" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="80" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B80" s="6" t="s">
+    <row r="81" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B81" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C80" s="6" t="s">
+      <c r="C81" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E80" s="3" t="s">
+      <c r="E81" s="3" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="81" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="A81" s="6" t="s">
+    <row r="82" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="A82" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B82" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C81" s="6" t="s">
+      <c r="C82" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="E81" s="9" t="s">
+      <c r="E82" s="9" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="82" spans="1:5" s="6" customFormat="1">
-      <c r="A82" s="7" t="s">
+    <row r="83" spans="1:5" s="6" customFormat="1">
+      <c r="A83" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B82" s="8"/>
-      <c r="C82" s="8"/>
-      <c r="D82" s="8"/>
-      <c r="E82" s="8"/>
-    </row>
-    <row r="83" spans="1:5" s="12" customFormat="1" ht="45">
-      <c r="A83" s="5"/>
-      <c r="B83" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="C83" s="5"/>
-      <c r="D83" s="5"/>
-      <c r="E83" s="4" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" s="12" customFormat="1" ht="30">
+      <c r="B83" s="8"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="8"/>
+      <c r="E83" s="8"/>
+    </row>
+    <row r="84" spans="1:5" s="12" customFormat="1" ht="45">
       <c r="A84" s="5"/>
       <c r="B84" s="20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
       <c r="E84" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="85" spans="1:5" s="12" customFormat="1" ht="30">
       <c r="A85" s="5"/>
       <c r="B85" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
       <c r="E85" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" s="12" customFormat="1" ht="45">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" s="12" customFormat="1" ht="30">
       <c r="A86" s="5"/>
       <c r="B86" s="20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
       <c r="E86" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" s="12" customFormat="1" ht="30">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" s="12" customFormat="1" ht="45">
       <c r="A87" s="5"/>
       <c r="B87" s="20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C87" s="5"/>
       <c r="D87" s="5"/>
       <c r="E87" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" s="6" customFormat="1" ht="45">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" s="12" customFormat="1" ht="30">
       <c r="A88" s="5"/>
       <c r="B88" s="20" t="s">
-        <v>94</v>
+        <v>167</v>
       </c>
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
       <c r="E88" s="4" t="s">
-        <v>120</v>
+        <v>172</v>
       </c>
     </row>
     <row r="89" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A89" s="5"/>
       <c r="B89" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
       <c r="E89" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" s="6" customFormat="1" ht="30">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="A90" s="5"/>
-      <c r="B90" s="5" t="s">
-        <v>68</v>
+      <c r="B90" s="20" t="s">
+        <v>95</v>
       </c>
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
       <c r="E90" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="A91" s="5"/>
+      <c r="B91" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5"/>
+      <c r="E91" s="4" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="91" spans="1:5" s="6" customFormat="1">
-      <c r="A91" s="7" t="s">
+    <row r="92" spans="1:5" s="6" customFormat="1">
+      <c r="A92" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B91" s="8"/>
-      <c r="C91" s="8"/>
-      <c r="D91" s="8"/>
-      <c r="E91" s="8"/>
-    </row>
-    <row r="92" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B92" s="6" t="s">
+      <c r="B92" s="8"/>
+      <c r="C92" s="8"/>
+      <c r="D92" s="8"/>
+      <c r="E92" s="8"/>
+    </row>
+    <row r="93" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B93" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C92" s="6" t="s">
+      <c r="C93" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="E92" s="3" t="s">
+      <c r="E93" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="93" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B93" s="4" t="s">
+    <row r="94" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B94" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="C93" s="6" t="s">
+      <c r="C94" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="E93" s="3" t="s">
+      <c r="E94" s="3" t="s">
         <v>205</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B94" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="C94" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="95" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B95" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="96" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B96" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B97" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="E96" s="3" t="s">
+      <c r="E97" s="3" t="s">
         <v>208</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" s="6" customFormat="1" ht="60">
-      <c r="B97" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="E97" s="3" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="98" spans="1:5" s="6" customFormat="1" ht="60">
       <c r="B98" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="99" spans="1:5" s="6" customFormat="1" ht="60">
       <c r="B99" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" s="6" customFormat="1" ht="60">
+      <c r="B100" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="E99" s="3" t="s">
+      <c r="E100" s="3" t="s">
         <v>211</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B100" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="C100" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="101" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B101" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="102" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B102" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
+      </c>
+      <c r="C102" s="6" t="s">
+        <v>194</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="103" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B103" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="104" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B104" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="105" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B105" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B106" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="E105" s="3" t="s">
+      <c r="E106" s="3" t="s">
         <v>217</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" s="6" customFormat="1" ht="45">
-      <c r="B106" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="E106" s="3" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="107" spans="1:5" s="6" customFormat="1" ht="45">
       <c r="B107" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" s="6" customFormat="1" ht="45">
+      <c r="B108" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="E107" s="3" t="s">
+      <c r="E108" s="3" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="108" spans="1:5" s="6" customFormat="1">
-      <c r="A108" s="7" t="s">
+    <row r="109" spans="1:5" s="6" customFormat="1">
+      <c r="A109" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="B108" s="8"/>
-      <c r="C108" s="8"/>
-      <c r="D108" s="8"/>
-      <c r="E108" s="8"/>
-    </row>
-    <row r="109" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B109" s="6" t="s">
+      <c r="B109" s="8"/>
+      <c r="C109" s="8"/>
+      <c r="D109" s="8"/>
+      <c r="E109" s="8"/>
+    </row>
+    <row r="110" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B110" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="E109" s="3" t="s">
+      <c r="E110" s="3" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="110" spans="1:5" s="6" customFormat="1" ht="30">
-      <c r="B110" s="4" t="s">
+    <row r="111" spans="1:5" s="6" customFormat="1" ht="30">
+      <c r="B111" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="E110" s="3" t="s">
+      <c r="E111" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="30">
-      <c r="A111" s="2" t="s">
+    <row r="112" spans="1:5" ht="30">
+      <c r="A112" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B111" s="18"/>
-      <c r="C111" s="18"/>
-      <c r="D111" s="14"/>
-      <c r="E111" s="19"/>
-    </row>
-    <row r="112" spans="1:5" s="15" customFormat="1" ht="30">
-      <c r="B112" s="15" t="s">
+      <c r="B112" s="18"/>
+      <c r="C112" s="18"/>
+      <c r="D112" s="14"/>
+      <c r="E112" s="19"/>
+    </row>
+    <row r="113" spans="2:5" s="15" customFormat="1" ht="30">
+      <c r="B113" s="15" t="s">
         <v>142</v>
-      </c>
-      <c r="D112" s="16"/>
-      <c r="E112" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="113" spans="2:5" s="15" customFormat="1" ht="45">
-      <c r="B113" s="15" t="s">
-        <v>143</v>
       </c>
       <c r="D113" s="16"/>
       <c r="E113" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="114" spans="2:5" s="15" customFormat="1" ht="45">
       <c r="B114" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D114" s="16"/>
       <c r="E114" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="115" spans="2:5" s="15" customFormat="1" ht="45">
       <c r="B115" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D115" s="16"/>
       <c r="E115" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="116" spans="2:5" s="15" customFormat="1" ht="45">
       <c r="B116" s="15" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D116" s="16"/>
       <c r="E116" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="117" spans="2:5" s="15" customFormat="1" ht="45">
       <c r="B117" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D117" s="16"/>
       <c r="E117" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5" s="15" customFormat="1" ht="45">
+      <c r="B118" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="D118" s="16"/>
+      <c r="E118" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="118" spans="2:5" s="6" customFormat="1">
-      <c r="E118" s="9"/>
-    </row>
-    <row r="119" spans="2:5" s="6" customFormat="1"/>
+    <row r="119" spans="2:5" s="6" customFormat="1">
+      <c r="E119" s="9"/>
+    </row>
     <row r="120" spans="2:5" s="6" customFormat="1"/>
     <row r="121" spans="2:5" s="6" customFormat="1"/>
     <row r="122" spans="2:5" s="6" customFormat="1"/>
@@ -4563,6 +4586,7 @@
     <row r="125" spans="2:5" s="6" customFormat="1"/>
     <row r="126" spans="2:5" s="6" customFormat="1"/>
     <row r="127" spans="2:5" s="6" customFormat="1"/>
+    <row r="128" spans="2:5" s="6" customFormat="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>